<commit_message>
Napojenie simulacie na gui, initView vyhodene
</commit_message>
<xml_diff>
--- a/Generovanie kodu.xlsx
+++ b/Generovanie kodu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrej Beliančin\Projects\DIS-SEM-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F37376-669F-4780-96E0-0BE482818522}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3761A86-F846-4162-A7F1-9F2BBF1A40B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAA8F1F5-8409-4114-88BB-3627D0CE125A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAA8F1F5-8409-4114-88BB-3627D0CE125A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD79F5DF-5EE7-4CA7-B719-F55D9FC90063}">
   <dimension ref="B1:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,7 +1359,7 @@
         <v>new Zastavka("CB",3900.0/310.0, this),</v>
       </c>
       <c r="K38" t="str">
-        <f t="shared" ref="K38:K45" si="3" xml:space="preserve"> "new ZastavkaLinky(" &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B38 &amp; CHAR(34) &amp; "), " &amp; D38 &amp; " * 60.0, " &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B39 &amp; CHAR(34) &amp; ")),"</f>
+        <f t="shared" ref="K38:K44" si="3" xml:space="preserve"> "new ZastavkaLinky(" &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B38 &amp; CHAR(34) &amp; "), " &amp; D38 &amp; " * 60.0, " &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B39 &amp; CHAR(34) &amp; ")),"</f>
         <v>new ZastavkaLinky(zastavky.get("CB"), 2.3 * 60.0, zastavky.get("K1")),</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Generovanie tabulky geeneratorov, casov...
</commit_message>
<xml_diff>
--- a/Generovanie kodu.xlsx
+++ b/Generovanie kodu.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrej Beliančin\Projects\DIS-SEM-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3761A86-F846-4162-A7F1-9F2BBF1A40B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA5BF2D-BE1A-4A1F-B2FF-BBC8962A3566}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CAA8F1F5-8409-4114-88BB-3627D0CE125A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CAA8F1F5-8409-4114-88BB-3627D0CE125A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hárok2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hárok3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="85">
   <si>
     <t>Linka A</t>
   </si>
@@ -147,18 +149,6 @@
     <t>CG</t>
   </si>
   <si>
-    <t>new Zastavka("K2",3900.0/210.0),</t>
-  </si>
-  <si>
-    <t>new Zastavka("K3",3900.0/220.0),</t>
-  </si>
-  <si>
-    <t>new Zastavka("K1",3900.0/260.0),</t>
-  </si>
-  <si>
-    <t>new Zastavka("ST",0.0),</t>
-  </si>
-  <si>
     <t xml:space="preserve">nazov kontajnera </t>
   </si>
   <si>
@@ -210,12 +200,6 @@
     <t>2.7</t>
   </si>
   <si>
-    <t>3.3</t>
-  </si>
-  <si>
-    <t>6.6</t>
-  </si>
-  <si>
     <t>0.5</t>
   </si>
   <si>
@@ -240,19 +224,70 @@
     <t>7.2</t>
   </si>
   <si>
-    <t>SUMA</t>
-  </si>
-  <si>
-    <t>new Zastavka("K1",3900.0/260.0, this),</t>
-  </si>
-  <si>
-    <t>new Zastavka("K2",3900.0/210.0, this),</t>
-  </si>
-  <si>
-    <t>new Zastavka("K3",3900.0/220.0, this),</t>
-  </si>
-  <si>
-    <t>new Zastavka("ST", 0.0, this),</t>
+    <t>new ZastavkaKonfiguracia("K1",260),</t>
+  </si>
+  <si>
+    <t>new ZastavkaKonfiguracia("K2", 210),</t>
+  </si>
+  <si>
+    <t>new ZastavkaKonfiguracia("K3", 220),</t>
+  </si>
+  <si>
+    <t>new ZastavkaKonfiguracia("ST",0),</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Zastavka</t>
+  </si>
+  <si>
+    <t>casPrichoduPrvehoZakaznika</t>
+  </si>
+  <si>
+    <t>casPrichoduPoslednehoZakaznika</t>
+  </si>
+  <si>
+    <t>Rozdiel</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>cas Prichodu Prveho Zakaznika</t>
+  </si>
+  <si>
+    <t>cas Prichodu Posledneho Zakaznika</t>
+  </si>
+  <si>
+    <t>Zaciatok zapasu</t>
+  </si>
+  <si>
+    <t>Súčet</t>
+  </si>
+  <si>
+    <t>Priemer</t>
+  </si>
+  <si>
+    <t>Medzisúčet</t>
+  </si>
+  <si>
+    <t>Počet</t>
+  </si>
+  <si>
+    <t>Pocet zakaznikov</t>
+  </si>
+  <si>
+    <t>doba jazdy</t>
+  </si>
+  <si>
+    <t>naspat</t>
+  </si>
+  <si>
+    <t>doba jazdy k stadionu</t>
   </si>
 </sst>
 </file>
@@ -277,7 +312,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -285,14 +320,103 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -609,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD79F5DF-5EE7-4CA7-B719-F55D9FC90063}">
   <dimension ref="B1:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:C32"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,14 +742,15 @@
     <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -639,364 +764,453 @@
         <v>17</v>
       </c>
       <c r="K2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="M2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3">
         <v>3.2</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>46</v>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="E3">
         <v>123</v>
       </c>
       <c r="G3" t="str">
-        <f>_xlfn.CONCAT("new Zastavka(",CHAR(34),B3,CHAR(34),",", "3900.0/", E3,".0",", this),")</f>
-        <v>new Zastavka("AA",3900.0/123.0, this),</v>
+        <f>_xlfn.CONCAT("new ZastavkaKonfiguracia(",CHAR(34),B3,CHAR(34),",",  E3,"),")</f>
+        <v>new ZastavkaKonfiguracia("AA",123),</v>
       </c>
       <c r="K3" t="str">
         <f xml:space="preserve"> "new ZastavkaLinky(" &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B3 &amp; CHAR(34) &amp; "), " &amp; D3 &amp; " * 60.0, " &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B4 &amp; CHAR(34) &amp; ")),"</f>
         <v>new ZastavkaLinky(zastavky.get("AA"), 3.2 * 60.0, zastavky.get("AB")),</v>
       </c>
-      <c r="T3" s="1"/>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="S3">
+        <f t="shared" ref="S3:S15" si="0">C3*60</f>
+        <v>192</v>
+      </c>
+      <c r="T3" s="2">
+        <f t="shared" ref="T3:T13" si="1">SUM(S3,T4)</f>
+        <v>2280</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>47</v>
+      <c r="D4" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="E4">
         <v>92</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" ref="G4:G45" si="0">_xlfn.CONCAT("new Zastavka(",CHAR(34),B4,CHAR(34),",", "3900.0/", E4,".0",", this),")</f>
-        <v>new Zastavka("AB",3900.0/92.0, this),</v>
+        <f t="shared" ref="G4:G16" si="2">_xlfn.CONCAT("new ZastavkaKonfiguracia(",CHAR(34),B4,CHAR(34),",",  E4,"),")</f>
+        <v>new ZastavkaKonfiguracia("AB",92),</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" ref="K4:K15" si="1" xml:space="preserve"> "new ZastavkaLinky(" &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B4 &amp; CHAR(34) &amp; "), " &amp; D4 &amp; " * 60.0, " &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B5 &amp; CHAR(34) &amp; ")),"</f>
+        <f t="shared" ref="K4:K15" si="3" xml:space="preserve"> "new ZastavkaLinky(" &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B4 &amp; CHAR(34) &amp; "), " &amp; D4 &amp; " * 60.0, " &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B5 &amp; CHAR(34) &amp; ")),"</f>
         <v>new ZastavkaLinky(zastavky.get("AB"), 2.3 * 60.0, zastavky.get("AC")),</v>
       </c>
-      <c r="T4" s="1"/>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="S4">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+      <c r="T4" s="2">
+        <f t="shared" si="1"/>
+        <v>2088</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5">
         <v>2.1</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>48</v>
+      <c r="D5" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="E5">
         <v>241</v>
       </c>
       <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>new ZastavkaKonfiguracia("AC",241),</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="3"/>
+        <v>new ZastavkaLinky(zastavky.get("AC"), 2.1 * 60.0, zastavky.get("AD")),</v>
+      </c>
+      <c r="S5">
         <f t="shared" si="0"/>
-        <v>new Zastavka("AC",3900.0/241.0, this),</v>
-      </c>
-      <c r="K5" t="str">
-        <f t="shared" si="1"/>
-        <v>new ZastavkaLinky(zastavky.get("AC"), 2.1 * 60.0, zastavky.get("AD")),</v>
-      </c>
-      <c r="T5" s="1"/>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="T5" s="2">
+        <f t="shared" si="1"/>
+        <v>1950</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
         <v>1.2</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>49</v>
+      <c r="D6" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="E6">
         <v>123</v>
       </c>
       <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>new ZastavkaKonfiguracia("AD",123),</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="3"/>
+        <v>new ZastavkaLinky(zastavky.get("AD"), 1.2 * 60.0, zastavky.get("K1")),</v>
+      </c>
+      <c r="S6">
         <f t="shared" si="0"/>
-        <v>new Zastavka("AD",3900.0/123.0, this),</v>
-      </c>
-      <c r="K6" t="str">
-        <f t="shared" si="1"/>
-        <v>new ZastavkaLinky(zastavky.get("AD"), 1.2 * 60.0, zastavky.get("K1")),</v>
-      </c>
-      <c r="T6" s="1"/>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="T6" s="2">
+        <f t="shared" si="1"/>
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
         <v>5.4</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>50</v>
+      <c r="D7" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="E7">
         <v>260</v>
       </c>
-      <c r="G7" t="str">
+      <c r="K7" t="str">
+        <f t="shared" si="3"/>
+        <v>new ZastavkaLinky(zastavky.get("K1"), 5.4 * 60.0, zastavky.get("AE")),</v>
+      </c>
+      <c r="S7">
         <f t="shared" si="0"/>
-        <v>new Zastavka("K1",3900.0/260.0, this),</v>
-      </c>
-      <c r="K7" t="str">
-        <f t="shared" si="1"/>
-        <v>new ZastavkaLinky(zastavky.get("K1"), 5.4 * 60.0, zastavky.get("AE")),</v>
-      </c>
-      <c r="T7" s="1"/>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+      <c r="T7" s="2">
+        <f t="shared" si="1"/>
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
         <v>2.9</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>51</v>
+      <c r="D8" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="E8">
         <v>215</v>
       </c>
       <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>new ZastavkaKonfiguracia("AE",215),</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="3"/>
+        <v>new ZastavkaLinky(zastavky.get("AE"), 2.9 * 60.0, zastavky.get("AF")),</v>
+      </c>
+      <c r="S8">
         <f t="shared" si="0"/>
-        <v>new Zastavka("AE",3900.0/215.0, this),</v>
-      </c>
-      <c r="K8" t="str">
-        <f t="shared" si="1"/>
-        <v>new ZastavkaLinky(zastavky.get("AE"), 2.9 * 60.0, zastavky.get("AF")),</v>
-      </c>
-      <c r="T8" s="1"/>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" si="1"/>
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
         <v>3.4</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>52</v>
+      <c r="D9" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="E9">
         <v>245</v>
       </c>
       <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>new ZastavkaKonfiguracia("AF",245),</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="3"/>
+        <v>new ZastavkaLinky(zastavky.get("AF"), 3.4 * 60.0, zastavky.get("AG")),</v>
+      </c>
+      <c r="S9">
         <f t="shared" si="0"/>
-        <v>new Zastavka("AF",3900.0/245.0, this),</v>
-      </c>
-      <c r="K9" t="str">
-        <f t="shared" si="1"/>
-        <v>new ZastavkaLinky(zastavky.get("AF"), 3.4 * 60.0, zastavky.get("AG")),</v>
-      </c>
-      <c r="T9" s="1"/>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="T9" s="2">
+        <f t="shared" si="1"/>
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
         <v>1.8</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>53</v>
+      <c r="D10" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="E10">
         <v>137</v>
       </c>
       <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>new ZastavkaKonfiguracia("AG",137),</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="3"/>
+        <v>new ZastavkaLinky(zastavky.get("AG"), 1.8 * 60.0, zastavky.get("K3")),</v>
+      </c>
+      <c r="S10">
         <f t="shared" si="0"/>
-        <v>new Zastavka("AG",3900.0/137.0, this),</v>
-      </c>
-      <c r="K10" t="str">
-        <f t="shared" si="1"/>
-        <v>new ZastavkaLinky(zastavky.get("AG"), 1.8 * 60.0, zastavky.get("K3")),</v>
-      </c>
-      <c r="T10" s="1"/>
-      <c r="U10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="T10" s="2">
+        <f t="shared" si="1"/>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>56</v>
+      <c r="D11" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="E11">
         <v>220</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>new ZastavkaLinky(zastavky.get("K3"), 4.0 * 60.0, zastavky.get("AH")),</v>
       </c>
-      <c r="U11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="S11">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="T11" s="2">
+        <f t="shared" si="1"/>
+        <v>942</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12">
         <v>1.6</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>54</v>
+      <c r="D12" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="E12">
         <v>132</v>
       </c>
       <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>new ZastavkaKonfiguracia("AH",132),</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="3"/>
+        <v>new ZastavkaLinky(zastavky.get("AH"), 1.6 * 60.0, zastavky.get("AI")),</v>
+      </c>
+      <c r="S12">
         <f t="shared" si="0"/>
-        <v>new Zastavka("AH",3900.0/132.0, this),</v>
-      </c>
-      <c r="K12" t="str">
-        <f t="shared" si="1"/>
-        <v>new ZastavkaLinky(zastavky.get("AH"), 1.6 * 60.0, zastavky.get("AI")),</v>
-      </c>
-      <c r="T12" s="1"/>
-      <c r="U12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="T12" s="2">
+        <f t="shared" si="1"/>
+        <v>702</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13">
         <v>4.5999999999999996</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>55</v>
+      <c r="D13" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="E13">
         <v>164</v>
       </c>
       <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>new ZastavkaKonfiguracia("AI",164),</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="3"/>
+        <v>new ZastavkaLinky(zastavky.get("AI"), 4.6 * 60.0, zastavky.get("AJ")),</v>
+      </c>
+      <c r="S13">
         <f t="shared" si="0"/>
-        <v>new Zastavka("AI",3900.0/164.0, this),</v>
-      </c>
-      <c r="K13" t="str">
-        <f t="shared" si="1"/>
-        <v>new ZastavkaLinky(zastavky.get("AI"), 4.6 * 60.0, zastavky.get("AJ")),</v>
-      </c>
-      <c r="T13" s="1"/>
-      <c r="U13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+      <c r="T13" s="2">
+        <f t="shared" si="1"/>
+        <v>606</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
         <v>3.4</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>52</v>
+      <c r="D14" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="E14">
         <v>124</v>
       </c>
       <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>new ZastavkaKonfiguracia("AJ",124),</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="3"/>
+        <v>new ZastavkaLinky(zastavky.get("AJ"), 3.4 * 60.0, zastavky.get("AK")),</v>
+      </c>
+      <c r="S14">
         <f t="shared" si="0"/>
-        <v>new Zastavka("AJ",3900.0/124.0, this),</v>
-      </c>
-      <c r="K14" t="str">
-        <f t="shared" si="1"/>
-        <v>new ZastavkaLinky(zastavky.get("AJ"), 3.4 * 60.0, zastavky.get("AK")),</v>
-      </c>
-      <c r="T14" s="1"/>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="T14" s="2">
+        <f>SUM(S14,T15)</f>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15">
         <v>1.2</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>49</v>
+      <c r="D15" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="E15">
         <v>213</v>
       </c>
       <c r="G15" t="str">
+        <f t="shared" si="2"/>
+        <v>new ZastavkaKonfiguracia("AK",213),</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="3"/>
+        <v>new ZastavkaLinky(zastavky.get("AK"), 1.2 * 60.0, zastavky.get("AL")),</v>
+      </c>
+      <c r="S15">
         <f t="shared" si="0"/>
-        <v>new Zastavka("AK",3900.0/213.0, this),</v>
-      </c>
-      <c r="K15" t="str">
-        <f t="shared" si="1"/>
-        <v>new ZastavkaLinky(zastavky.get("AK"), 1.2 * 60.0, zastavky.get("AL")),</v>
-      </c>
-      <c r="T15" s="1"/>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="T15" s="2">
+        <f>SUM(S15:S16)</f>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16">
         <v>0.9</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>45</v>
+      <c r="D16" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="E16">
         <v>185</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("AL",3900.0/185.0, this),</v>
+        <f t="shared" si="2"/>
+        <v>new ZastavkaKonfiguracia("AL",185),</v>
       </c>
       <c r="K16" t="str">
         <f xml:space="preserve"> "new ZastavkaLinky(" &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B16 &amp; CHAR(34) &amp; "), " &amp; D16 &amp; " * 60.0, " &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B17 &amp; CHAR(34) &amp; "))"</f>
         <v>new ZastavkaLinky(zastavky.get("AL"), 0.9 * 60.0, zastavky.get("ST"))</v>
       </c>
+      <c r="S16">
+        <f>C16*60</f>
+        <v>54</v>
+      </c>
+      <c r="T16" s="2"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" t="s">
-        <v>69</v>
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>25</v>
       </c>
       <c r="D17">
-        <f>SUM(C3:C16)</f>
-        <v>38</v>
-      </c>
-      <c r="G17" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("ST",3900.0/.0, this),</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="K17" t="str">
+        <f xml:space="preserve"> "new ZastavkaLinky(" &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B17 &amp; CHAR(34) &amp; "), " &amp; D17 &amp; " * 60.0, " &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B18 &amp; CHAR(34) &amp; "))"</f>
+        <v>new ZastavkaLinky(zastavky.get("ST"), 25 * 60.0, zastavky.get("AA"))</v>
+      </c>
+      <c r="T17" s="2"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="D18" s="2"/>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="T18" s="2"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="1"/>
+      <c r="T19" s="2"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
@@ -1005,10 +1219,11 @@
       <c r="C20" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="1"/>
       <c r="E20" t="s">
         <v>18</v>
       </c>
+      <c r="T20" s="2"/>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
@@ -1017,18 +1232,18 @@
       <c r="C21">
         <v>1.2</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>49</v>
+      <c r="D21" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="E21">
         <v>79</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("BA",3900.0/79.0, this),</v>
+        <f t="shared" ref="G21:G32" si="4">_xlfn.CONCAT("new ZastavkaKonfiguracia(",CHAR(34),B21,CHAR(34),",",  E21,"),")</f>
+        <v>new ZastavkaKonfiguracia("BA",79),</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" ref="K21:K31" si="2" xml:space="preserve"> "new ZastavkaLinky(" &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B21 &amp; CHAR(34) &amp; "), " &amp; D21 &amp; " * 60.0, " &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B22 &amp; CHAR(34) &amp; ")),"</f>
+        <f t="shared" ref="K21:K31" si="5" xml:space="preserve"> "new ZastavkaLinky(" &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B21 &amp; CHAR(34) &amp; "), " &amp; D21 &amp; " * 60.0, " &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B22 &amp; CHAR(34) &amp; ")),"</f>
         <v>new ZastavkaLinky(zastavky.get("BA"), 1.2 * 60.0, zastavky.get("BB")),</v>
       </c>
     </row>
@@ -1039,18 +1254,18 @@
       <c r="C22">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>47</v>
+      <c r="D22" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="E22">
         <v>69</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("BB",3900.0/69.0, this),</v>
+        <f t="shared" si="4"/>
+        <v>new ZastavkaKonfiguracia("BB",69),</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>new ZastavkaLinky(zastavky.get("BB"), 2.3 * 60.0, zastavky.get("BC")),</v>
       </c>
     </row>
@@ -1061,22 +1276,22 @@
       <c r="C23">
         <v>3.2</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>46</v>
+      <c r="D23" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="E23">
         <v>43</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("BC",3900.0/43.0, this),</v>
+        <f t="shared" si="4"/>
+        <v>new ZastavkaKonfiguracia("BC",43),</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>new ZastavkaLinky(zastavky.get("BC"), 3.2 * 60.0, zastavky.get("BD")),</v>
       </c>
       <c r="U23" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.25">
@@ -1086,22 +1301,22 @@
       <c r="C24">
         <v>4.3</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>57</v>
+      <c r="D24" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="E24">
         <v>127</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("BD",3900.0/127.0, this),</v>
+        <f t="shared" si="4"/>
+        <v>new ZastavkaKonfiguracia("BD",127),</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>new ZastavkaLinky(zastavky.get("BD"), 4.3 * 60.0, zastavky.get("K2")),</v>
       </c>
       <c r="U24" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.25">
@@ -1111,22 +1326,18 @@
       <c r="C25">
         <v>1.2</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>49</v>
+      <c r="D25" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="E25">
         <v>210</v>
       </c>
-      <c r="G25" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("K2",3900.0/210.0, this),</v>
-      </c>
       <c r="K25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>new ZastavkaLinky(zastavky.get("K2"), 1.2 * 60.0, zastavky.get("BE")),</v>
       </c>
       <c r="U25" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.25">
@@ -1136,22 +1347,22 @@
       <c r="C26">
         <v>2.7</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>58</v>
+      <c r="D26" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="E26">
         <v>30</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("BE",3900.0/30.0, this),</v>
+        <f t="shared" si="4"/>
+        <v>new ZastavkaKonfiguracia("BE",30),</v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>new ZastavkaLinky(zastavky.get("BE"), 2.7 * 60.0, zastavky.get("BF")),</v>
       </c>
       <c r="U26" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.25">
@@ -1161,19 +1372,19 @@
       <c r="C27">
         <v>3</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>59</v>
+      <c r="D27" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="E27">
         <v>69</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("BF",3900.0/69.0, this),</v>
+        <f t="shared" si="4"/>
+        <v>new ZastavkaKonfiguracia("BF",69),</v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="2"/>
-        <v>new ZastavkaLinky(zastavky.get("BF"), 3.3 * 60.0, zastavky.get("K3")),</v>
+        <f t="shared" si="5"/>
+        <v>new ZastavkaLinky(zastavky.get("BF"), 3 * 60.0, zastavky.get("K3")),</v>
       </c>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.25">
@@ -1183,19 +1394,15 @@
       <c r="C28">
         <v>6</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>60</v>
+      <c r="D28" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="E28">
         <v>220</v>
       </c>
-      <c r="G28" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("K3",3900.0/220.0, this),</v>
-      </c>
       <c r="K28" t="str">
-        <f t="shared" si="2"/>
-        <v>new ZastavkaLinky(zastavky.get("K3"), 6.6 * 60.0, zastavky.get("BG")),</v>
+        <f t="shared" si="5"/>
+        <v>new ZastavkaLinky(zastavky.get("K3"), 6 * 60.0, zastavky.get("BG")),</v>
       </c>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.25">
@@ -1205,18 +1412,18 @@
       <c r="C29">
         <v>4.3</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>57</v>
+      <c r="D29" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="E29">
         <v>162</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("BG",3900.0/162.0, this),</v>
+        <f t="shared" si="4"/>
+        <v>new ZastavkaKonfiguracia("BG",162),</v>
       </c>
       <c r="K29" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>new ZastavkaLinky(zastavky.get("BG"), 4.3 * 60.0, zastavky.get("BH")),</v>
       </c>
     </row>
@@ -1227,18 +1434,18 @@
       <c r="C30">
         <v>0.5</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>61</v>
+      <c r="D30" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="E30">
         <v>90</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("BH",3900.0/90.0, this),</v>
+        <f t="shared" si="4"/>
+        <v>new ZastavkaKonfiguracia("BH",90),</v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>new ZastavkaLinky(zastavky.get("BH"), 0.5 * 60.0, zastavky.get("BI")),</v>
       </c>
     </row>
@@ -1249,18 +1456,18 @@
       <c r="C31">
         <v>2.7</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>58</v>
+      <c r="D31" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="E31">
         <v>148</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("BI",3900.0/148.0, this),</v>
+        <f t="shared" si="4"/>
+        <v>new ZastavkaKonfiguracia("BI",148),</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>new ZastavkaLinky(zastavky.get("BI"), 2.7 * 60.0, zastavky.get("BJ")),</v>
       </c>
     </row>
@@ -1271,261 +1478,2276 @@
       <c r="C32">
         <v>1.3</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>62</v>
+      <c r="D32" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="E32">
         <v>171</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("BJ",3900.0/171.0, this),</v>
+        <f t="shared" si="4"/>
+        <v>new ZastavkaKonfiguracia("BJ",171),</v>
       </c>
       <c r="K32" t="str">
         <f xml:space="preserve"> "new ZastavkaLinky(" &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B32 &amp; CHAR(34) &amp; "), " &amp; D32 &amp; " * 60.0, " &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B33 &amp; CHAR(34) &amp; "))"</f>
         <v>new ZastavkaLinky(zastavky.get("BJ"), 1.3 * 60.0, zastavky.get("ST"))</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" t="s">
-        <v>69</v>
+        <v>40</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
       </c>
       <c r="D33">
-        <f>SUM(C21:C32)</f>
-        <v>32.699999999999996</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="K33" t="str">
+        <f xml:space="preserve"> "new ZastavkaLinky(" &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B33 &amp; CHAR(34) &amp; "), " &amp; D33 &amp; " * 60.0, " &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B34 &amp; CHAR(34) &amp; "))"</f>
+        <v>new ZastavkaLinky(zastavky.get("ST"), 10 * 60.0, zastavky.get("BA"))</v>
+      </c>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>19</v>
       </c>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>1</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="D36" s="1"/>
       <c r="E36" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>31</v>
       </c>
       <c r="C37">
         <v>0.6</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>63</v>
+      <c r="D37" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="E37">
         <v>240</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("CA",3900.0/240.0, this),</v>
+        <f t="shared" ref="G37:G38" si="6">_xlfn.CONCAT("new ZastavkaKonfiguracia(",CHAR(34),B37,CHAR(34),",",  E37,"),")</f>
+        <v>new ZastavkaKonfiguracia("CA",240),</v>
       </c>
       <c r="K37" t="str">
         <f xml:space="preserve"> "new ZastavkaLinky(" &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B37 &amp; CHAR(34) &amp; "), " &amp; D37 &amp; " * 60.0, " &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B38 &amp; CHAR(34) &amp; ")),"</f>
         <v>new ZastavkaLinky(zastavky.get("CA"), 0.6 * 60.0, zastavky.get("CB")),</v>
       </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="S37">
+        <f>C37*60</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>32</v>
       </c>
       <c r="C38">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>47</v>
+      <c r="D38" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="E38">
         <v>310</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("CB",3900.0/310.0, this),</v>
+        <f t="shared" si="6"/>
+        <v>new ZastavkaKonfiguracia("CB",310),</v>
       </c>
       <c r="K38" t="str">
-        <f t="shared" ref="K38:K44" si="3" xml:space="preserve"> "new ZastavkaLinky(" &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B38 &amp; CHAR(34) &amp; "), " &amp; D38 &amp; " * 60.0, " &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B39 &amp; CHAR(34) &amp; ")),"</f>
+        <f t="shared" ref="K38:K45" si="7" xml:space="preserve"> "new ZastavkaLinky(" &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B38 &amp; CHAR(34) &amp; "), " &amp; D38 &amp; " * 60.0, " &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B39 &amp; CHAR(34) &amp; ")),"</f>
         <v>new ZastavkaLinky(zastavky.get("CB"), 2.3 * 60.0, zastavky.get("K1")),</v>
       </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="S38">
+        <f t="shared" ref="S38:S45" si="8">C38*60</f>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>7</v>
       </c>
       <c r="C39">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>64</v>
+      <c r="D39" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="E39">
         <v>260</v>
       </c>
       <c r="K39" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>new ZastavkaLinky(zastavky.get("K1"), 4.1 * 60.0, zastavky.get("K2")),</v>
       </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="S39">
+        <f t="shared" si="8"/>
+        <v>245.99999999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>24</v>
       </c>
       <c r="C40">
         <v>6</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>60</v>
+      <c r="D40" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="E40">
         <v>210</v>
       </c>
       <c r="K40" t="str">
-        <f t="shared" si="3"/>
-        <v>new ZastavkaLinky(zastavky.get("K2"), 6.6 * 60.0, zastavky.get("CC")),</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>new ZastavkaLinky(zastavky.get("K2"), 6 * 60.0, zastavky.get("CC")),</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="8"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>33</v>
       </c>
       <c r="C41">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>47</v>
+      <c r="D41" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="E41">
         <v>131</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("CC",3900.0/131.0, this),</v>
+        <f t="shared" ref="G41:G45" si="9">_xlfn.CONCAT("new ZastavkaKonfiguracia(",CHAR(34),B41,CHAR(34),",",  E41,"),")</f>
+        <v>new ZastavkaKonfiguracia("CC",131),</v>
       </c>
       <c r="K41" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>new ZastavkaLinky(zastavky.get("CC"), 2.3 * 60.0, zastavky.get("CD")),</v>
       </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="S41">
+        <f t="shared" si="8"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>34</v>
       </c>
       <c r="C42">
         <v>7.1</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>65</v>
+      <c r="D42" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="E42">
         <v>190</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("CD",3900.0/190.0, this),</v>
+        <f t="shared" si="9"/>
+        <v>new ZastavkaKonfiguracia("CD",190),</v>
       </c>
       <c r="K42" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>new ZastavkaLinky(zastavky.get("CD"), 7.1 * 60.0, zastavky.get("CE")),</v>
       </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="S42">
+        <f t="shared" si="8"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="43" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>35</v>
       </c>
       <c r="C43">
         <v>4.8</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>66</v>
+      <c r="D43" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="E43">
         <v>132</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("CE",3900.0/132.0, this),</v>
+        <f t="shared" si="9"/>
+        <v>new ZastavkaKonfiguracia("CE",132),</v>
       </c>
       <c r="K43" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>new ZastavkaLinky(zastavky.get("CE"), 4.8 * 60.0, zastavky.get("CF")),</v>
       </c>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="S43">
+        <f t="shared" si="8"/>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>36</v>
       </c>
       <c r="C44">
         <v>3.7</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>67</v>
+      <c r="D44" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="E44">
         <v>128</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("CF",3900.0/128.0, this),</v>
+        <f t="shared" si="9"/>
+        <v>new ZastavkaKonfiguracia("CF",128),</v>
       </c>
       <c r="K44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>new ZastavkaLinky(zastavky.get("CF"), 3.7 * 60.0, zastavky.get("CG")),</v>
       </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="S44">
+        <f t="shared" si="8"/>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="45" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>37</v>
       </c>
       <c r="C45">
         <v>7.2</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>68</v>
+      <c r="D45" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="E45">
         <v>70</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="0"/>
-        <v>new Zastavka("CG",3900.0/70.0, this),</v>
+        <f t="shared" si="9"/>
+        <v>new ZastavkaKonfiguracia("CG",70),</v>
       </c>
       <c r="K45" t="str">
-        <f xml:space="preserve"> "new ZastavkaLinky(" &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B45 &amp; CHAR(34) &amp; "), " &amp; D45 &amp; " * 60.0, " &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B46 &amp; CHAR(34) &amp; "))"</f>
-        <v>new ZastavkaLinky(zastavky.get("CG"), 7.2 * 60.0, zastavky.get("ST"))</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>new ZastavkaLinky(zastavky.get("CG"), 7.2 * 60.0, zastavky.get("ST")),</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="8"/>
+        <v>432</v>
+      </c>
+    </row>
+    <row r="46" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>44</v>
-      </c>
-      <c r="C46" t="s">
-        <v>69</v>
+        <v>40</v>
+      </c>
+      <c r="C46">
+        <v>30</v>
       </c>
       <c r="D46">
-        <f>SUM(C37:C45)</f>
-        <v>38.1</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D47" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="K46" t="str">
+        <f xml:space="preserve"> "new ZastavkaLinky(" &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B46 &amp; CHAR(34) &amp; "), " &amp; D46 &amp; " * 60.0, " &amp; $M$2 &amp; ".get(" &amp; CHAR(34) &amp; B47 &amp; CHAR(34) &amp; "))"</f>
+        <v>new ZastavkaLinky(zastavky.get("ST"), 30 * 60.0, zastavky.get("CA"))</v>
+      </c>
+      <c r="S46">
+        <f>SUM(S37:S45)</f>
+        <v>2286</v>
+      </c>
+    </row>
+    <row r="47" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C15344-21F8-4E67-A098-0EABFA05ED44}">
+  <dimension ref="A1:U44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" sqref="G14:G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="7" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27" customWidth="1"/>
+    <col min="12" max="12" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.42578125" customWidth="1"/>
+    <col min="14" max="14" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1">
+        <v>6786</v>
+      </c>
+      <c r="M1">
+        <f>B1/60</f>
+        <v>113.1</v>
+      </c>
+      <c r="N1">
+        <f>M1/60</f>
+        <v>1.885</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L2" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>396</v>
+      </c>
+      <c r="C3">
+        <v>4296</v>
+      </c>
+      <c r="D3">
+        <v>3900</v>
+      </c>
+      <c r="E3">
+        <v>56.521739130434703</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>3.2</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I13" si="0">I4+H3</f>
+        <v>37.999999999999993</v>
+      </c>
+      <c r="J3" s="4">
+        <v>6</v>
+      </c>
+      <c r="K3" s="4">
+        <f>J3/60</f>
+        <v>0.1</v>
+      </c>
+      <c r="L3" s="4">
+        <v>3906</v>
+      </c>
+      <c r="M3" s="5">
+        <f>L3/60</f>
+        <v>65.099999999999994</v>
+      </c>
+      <c r="N3">
+        <v>3900</v>
+      </c>
+      <c r="O3">
+        <v>31.707317073170699</v>
+      </c>
+      <c r="P3">
+        <f>N3/O3</f>
+        <v>123.00000000000013</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>534</v>
+      </c>
+      <c r="C4">
+        <v>4434</v>
+      </c>
+      <c r="D4">
+        <v>3900</v>
+      </c>
+      <c r="E4">
+        <v>90.697674418604606</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>34.79999999999999</v>
+      </c>
+      <c r="J4" s="7">
+        <v>198</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" ref="K4:K40" si="1">J4/60</f>
+        <v>3.3</v>
+      </c>
+      <c r="L4" s="7">
+        <v>4098</v>
+      </c>
+      <c r="M4" s="8">
+        <f t="shared" ref="M4:M40" si="2">L4/60</f>
+        <v>68.3</v>
+      </c>
+      <c r="N4">
+        <v>3900</v>
+      </c>
+      <c r="O4">
+        <v>42.391304347826001</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P40" si="3">N4/O4</f>
+        <v>92.000000000000185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>726</v>
+      </c>
+      <c r="C5">
+        <v>4626</v>
+      </c>
+      <c r="D5">
+        <v>3900</v>
+      </c>
+      <c r="E5">
+        <v>30.708661417322801</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>2.1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>32.499999999999993</v>
+      </c>
+      <c r="J5" s="7">
+        <v>336</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" si="1"/>
+        <v>5.6</v>
+      </c>
+      <c r="L5" s="7">
+        <v>4236</v>
+      </c>
+      <c r="M5" s="8">
+        <f t="shared" si="2"/>
+        <v>70.599999999999994</v>
+      </c>
+      <c r="N5">
+        <v>3900</v>
+      </c>
+      <c r="O5">
+        <v>16.182572614107801</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="3"/>
+        <v>241.00000000000122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>1056</v>
+      </c>
+      <c r="C6">
+        <v>4956</v>
+      </c>
+      <c r="D6">
+        <v>3900</v>
+      </c>
+      <c r="E6">
+        <v>130</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6">
+        <v>1.2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>30.399999999999995</v>
+      </c>
+      <c r="J6" s="7">
+        <v>462</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="1"/>
+        <v>7.7</v>
+      </c>
+      <c r="L6" s="7">
+        <v>4362</v>
+      </c>
+      <c r="M6" s="8">
+        <f t="shared" si="2"/>
+        <v>72.7</v>
+      </c>
+      <c r="N6">
+        <v>3900</v>
+      </c>
+      <c r="O6">
+        <v>31.707317073170699</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="3"/>
+        <v>123.00000000000013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>5.4</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>29.199999999999996</v>
+      </c>
+      <c r="J7">
+        <v>174</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>2.9</v>
+      </c>
+      <c r="L7">
+        <v>4434</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>73.900000000000006</v>
+      </c>
+      <c r="P7">
+        <f>P38/2</f>
+        <v>130.00000000000065</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>1218</v>
+      </c>
+      <c r="C8">
+        <v>5118</v>
+      </c>
+      <c r="D8">
+        <v>3900</v>
+      </c>
+      <c r="E8">
+        <v>56.521739130434703</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <v>2.9</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>23.799999999999997</v>
+      </c>
+      <c r="J8" s="7">
+        <v>858</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="1"/>
+        <v>14.3</v>
+      </c>
+      <c r="L8" s="7">
+        <v>4758</v>
+      </c>
+      <c r="M8" s="8">
+        <f t="shared" si="2"/>
+        <v>79.3</v>
+      </c>
+      <c r="N8">
+        <v>3900</v>
+      </c>
+      <c r="O8">
+        <v>18.139534883720899</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="3"/>
+        <v>215.00000000000037</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9">
+        <v>1758</v>
+      </c>
+      <c r="C9">
+        <v>5658</v>
+      </c>
+      <c r="D9">
+        <v>3900</v>
+      </c>
+      <c r="E9">
+        <v>24.074074074074002</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>3.4</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>20.9</v>
+      </c>
+      <c r="J9" s="7">
+        <v>1032</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="1"/>
+        <v>17.2</v>
+      </c>
+      <c r="L9" s="7">
+        <v>4932</v>
+      </c>
+      <c r="M9" s="8">
+        <f t="shared" si="2"/>
+        <v>82.2</v>
+      </c>
+      <c r="N9">
+        <v>3900</v>
+      </c>
+      <c r="O9">
+        <v>15.9183673469387</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="3"/>
+        <v>245.00000000000117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>2016</v>
+      </c>
+      <c r="C10">
+        <v>5916</v>
+      </c>
+      <c r="D10">
+        <v>3900</v>
+      </c>
+      <c r="E10">
+        <v>43.3333333333333</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <v>1.8</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="J10" s="7">
+        <v>1236</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="1"/>
+        <v>20.6</v>
+      </c>
+      <c r="L10" s="7">
+        <v>5136</v>
+      </c>
+      <c r="M10" s="8">
+        <f t="shared" si="2"/>
+        <v>85.6</v>
+      </c>
+      <c r="N10">
+        <v>3900</v>
+      </c>
+      <c r="O10">
+        <v>28.4671532846715</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="3"/>
+        <v>137.00000000000017</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>15.7</v>
+      </c>
+      <c r="J11">
+        <v>1344</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>22.4</v>
+      </c>
+      <c r="L11">
+        <v>5298</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>88.3</v>
+      </c>
+      <c r="P11">
+        <f>P40/2</f>
+        <v>110.00000000000044</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>174</v>
+      </c>
+      <c r="C12">
+        <v>4434</v>
+      </c>
+      <c r="D12">
+        <v>4260</v>
+      </c>
+      <c r="E12">
+        <v>16.384615384615302</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12">
+        <v>1.6</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>11.7</v>
+      </c>
+      <c r="J12" s="7">
+        <v>1584</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="1"/>
+        <v>26.4</v>
+      </c>
+      <c r="L12" s="7">
+        <v>5484</v>
+      </c>
+      <c r="M12" s="8">
+        <f t="shared" si="2"/>
+        <v>91.4</v>
+      </c>
+      <c r="N12">
+        <v>3900</v>
+      </c>
+      <c r="O12">
+        <v>29.545454545454501</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="3"/>
+        <v>132.0000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <v>2046</v>
+      </c>
+      <c r="C13">
+        <v>5946</v>
+      </c>
+      <c r="D13">
+        <v>3900</v>
+      </c>
+      <c r="E13">
+        <v>26.351351351351301</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>10.1</v>
+      </c>
+      <c r="J13" s="7">
+        <v>1680</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="L13" s="7">
+        <v>5580</v>
+      </c>
+      <c r="M13" s="8">
+        <f t="shared" si="2"/>
+        <v>93</v>
+      </c>
+      <c r="N13">
+        <v>3900</v>
+      </c>
+      <c r="O13">
+        <v>23.780487804878</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="3"/>
+        <v>164.00000000000034</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <v>420</v>
+      </c>
+      <c r="C14">
+        <v>4884</v>
+      </c>
+      <c r="D14">
+        <v>4464</v>
+      </c>
+      <c r="E14">
+        <v>21.257142857142799</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14">
+        <v>3.4</v>
+      </c>
+      <c r="I14">
+        <f>I15+H14</f>
+        <v>5.5</v>
+      </c>
+      <c r="J14" s="7">
+        <v>1956</v>
+      </c>
+      <c r="K14" s="7">
+        <f t="shared" si="1"/>
+        <v>32.6</v>
+      </c>
+      <c r="L14" s="7">
+        <v>5856</v>
+      </c>
+      <c r="M14" s="8">
+        <f t="shared" si="2"/>
+        <v>97.6</v>
+      </c>
+      <c r="N14">
+        <v>3900</v>
+      </c>
+      <c r="O14">
+        <v>31.451612903225801</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="3"/>
+        <v>124.00000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>2208</v>
+      </c>
+      <c r="C15">
+        <v>6108</v>
+      </c>
+      <c r="D15">
+        <v>3900</v>
+      </c>
+      <c r="E15">
+        <v>22.807017543859601</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15">
+        <v>1.2</v>
+      </c>
+      <c r="I15">
+        <f>I16+H15</f>
+        <v>2.1</v>
+      </c>
+      <c r="J15" s="7">
+        <v>2160</v>
+      </c>
+      <c r="K15" s="7">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="L15" s="7">
+        <v>6060</v>
+      </c>
+      <c r="M15" s="8">
+        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
+      <c r="N15">
+        <v>3900</v>
+      </c>
+      <c r="O15">
+        <v>18.309859154929502</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="3"/>
+        <v>213.00000000000088</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>1344</v>
+      </c>
+      <c r="C16">
+        <v>5298</v>
+      </c>
+      <c r="D16">
+        <v>3954</v>
+      </c>
+      <c r="E16">
+        <v>17.972727272727202</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16">
+        <v>0.9</v>
+      </c>
+      <c r="I16">
+        <f>H16</f>
+        <v>0.9</v>
+      </c>
+      <c r="J16" s="10">
+        <v>2232</v>
+      </c>
+      <c r="K16" s="10">
+        <f t="shared" si="1"/>
+        <v>37.200000000000003</v>
+      </c>
+      <c r="L16" s="10">
+        <v>6132</v>
+      </c>
+      <c r="M16" s="11">
+        <f t="shared" si="2"/>
+        <v>102.2</v>
+      </c>
+      <c r="N16">
+        <v>3900</v>
+      </c>
+      <c r="O16">
+        <v>21.081081081080999</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="3"/>
+        <v>185.00000000000071</v>
+      </c>
+      <c r="Q16">
+        <f>SUM(P3:P16)</f>
+        <v>2234.0000000000068</v>
+      </c>
+      <c r="R16" t="s">
+        <v>83</v>
+      </c>
+      <c r="S16">
+        <v>25</v>
+      </c>
+      <c r="U16">
+        <f>Q16/186</f>
+        <v>12.010752688172079</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>3900</v>
+      </c>
+      <c r="D17">
+        <v>3900</v>
+      </c>
+      <c r="E17">
+        <v>16.25</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17">
+        <v>1.2</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ref="I17:I26" si="4">I18+H17</f>
+        <v>32.700000000000003</v>
+      </c>
+      <c r="J17" s="4">
+        <v>324</v>
+      </c>
+      <c r="K17" s="4">
+        <f t="shared" si="1"/>
+        <v>5.4</v>
+      </c>
+      <c r="L17" s="4">
+        <v>4224</v>
+      </c>
+      <c r="M17" s="5">
+        <f t="shared" si="2"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="N17">
+        <v>3900</v>
+      </c>
+      <c r="O17">
+        <v>49.367088607594901</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="3"/>
+        <v>79.000000000000057</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>36</v>
+      </c>
+      <c r="C18">
+        <v>3936</v>
+      </c>
+      <c r="D18">
+        <v>3900</v>
+      </c>
+      <c r="E18">
+        <v>12.580645161290301</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="4"/>
+        <v>31.5</v>
+      </c>
+      <c r="J18" s="7">
+        <v>396</v>
+      </c>
+      <c r="K18" s="7">
+        <f t="shared" si="1"/>
+        <v>6.6</v>
+      </c>
+      <c r="L18" s="7">
+        <v>4296</v>
+      </c>
+      <c r="M18" s="8">
+        <f t="shared" si="2"/>
+        <v>71.599999999999994</v>
+      </c>
+      <c r="N18">
+        <v>3900</v>
+      </c>
+      <c r="O18">
+        <v>56.521739130434703</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="3"/>
+        <v>69.000000000000099</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>3906</v>
+      </c>
+      <c r="D19">
+        <v>3900</v>
+      </c>
+      <c r="E19">
+        <v>31.707317073170699</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19">
+        <v>3.2</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="4"/>
+        <v>29.2</v>
+      </c>
+      <c r="J19" s="7">
+        <v>534</v>
+      </c>
+      <c r="K19" s="7">
+        <f t="shared" si="1"/>
+        <v>8.9</v>
+      </c>
+      <c r="L19" s="7">
+        <v>4434</v>
+      </c>
+      <c r="M19" s="8">
+        <f t="shared" si="2"/>
+        <v>73.900000000000006</v>
+      </c>
+      <c r="N19">
+        <v>3900</v>
+      </c>
+      <c r="O19">
+        <v>90.697674418604606</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="3"/>
+        <v>43.000000000000021</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20">
+        <v>780</v>
+      </c>
+      <c r="C20">
+        <v>4680</v>
+      </c>
+      <c r="D20">
+        <v>3900</v>
+      </c>
+      <c r="E20">
+        <v>29.770992366412202</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20">
+        <v>4.3</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="J20" s="7">
+        <v>726</v>
+      </c>
+      <c r="K20" s="7">
+        <f t="shared" si="1"/>
+        <v>12.1</v>
+      </c>
+      <c r="L20" s="7">
+        <v>4626</v>
+      </c>
+      <c r="M20" s="8">
+        <f t="shared" si="2"/>
+        <v>77.099999999999994</v>
+      </c>
+      <c r="N20">
+        <v>3900</v>
+      </c>
+      <c r="O20">
+        <v>30.708661417322801</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="3"/>
+        <v>127.00000000000014</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21">
+        <v>1.2</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="4"/>
+        <v>21.7</v>
+      </c>
+      <c r="J21">
+        <v>420</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="L21">
+        <v>4884</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="2"/>
+        <v>81.400000000000006</v>
+      </c>
+      <c r="P21">
+        <f>P39/2</f>
+        <v>105.00000000000028</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>198</v>
+      </c>
+      <c r="C22">
+        <v>4098</v>
+      </c>
+      <c r="D22">
+        <v>3900</v>
+      </c>
+      <c r="E22">
+        <v>42.391304347826001</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22">
+        <v>2.7</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="4"/>
+        <v>20.5</v>
+      </c>
+      <c r="J22" s="7">
+        <v>1056</v>
+      </c>
+      <c r="K22" s="7">
+        <f t="shared" si="1"/>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="L22" s="7">
+        <v>4956</v>
+      </c>
+      <c r="M22" s="8">
+        <f t="shared" si="2"/>
+        <v>82.6</v>
+      </c>
+      <c r="N22">
+        <v>3900</v>
+      </c>
+      <c r="O22">
+        <v>130</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23">
+        <v>918</v>
+      </c>
+      <c r="C23">
+        <v>4818</v>
+      </c>
+      <c r="D23">
+        <v>3900</v>
+      </c>
+      <c r="E23">
+        <v>20.5263157894736</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="4"/>
+        <v>17.8</v>
+      </c>
+      <c r="J23" s="7">
+        <v>1218</v>
+      </c>
+      <c r="K23" s="7">
+        <f t="shared" si="1"/>
+        <v>20.3</v>
+      </c>
+      <c r="L23" s="7">
+        <v>5118</v>
+      </c>
+      <c r="M23" s="8">
+        <f t="shared" si="2"/>
+        <v>85.3</v>
+      </c>
+      <c r="N23">
+        <v>3900</v>
+      </c>
+      <c r="O23">
+        <v>56.521739130434703</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="3"/>
+        <v>69.000000000000099</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24">
+        <v>6</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="4"/>
+        <v>14.8</v>
+      </c>
+      <c r="J24">
+        <v>1344</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>22.4</v>
+      </c>
+      <c r="L24">
+        <v>5298</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="2"/>
+        <v>88.3</v>
+      </c>
+      <c r="P24">
+        <f>P40/2</f>
+        <v>110.00000000000044</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>336</v>
+      </c>
+      <c r="C25">
+        <v>4236</v>
+      </c>
+      <c r="D25">
+        <v>3900</v>
+      </c>
+      <c r="E25">
+        <v>16.182572614107801</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25">
+        <v>4.3</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="4"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J25" s="7">
+        <v>1758</v>
+      </c>
+      <c r="K25" s="7">
+        <f t="shared" si="1"/>
+        <v>29.3</v>
+      </c>
+      <c r="L25" s="7">
+        <v>5658</v>
+      </c>
+      <c r="M25" s="8">
+        <f t="shared" si="2"/>
+        <v>94.3</v>
+      </c>
+      <c r="N25">
+        <v>3900</v>
+      </c>
+      <c r="O25">
+        <v>24.074074074074002</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="3"/>
+        <v>162.00000000000048</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26">
+        <v>1344</v>
+      </c>
+      <c r="C26">
+        <v>5244</v>
+      </c>
+      <c r="D26">
+        <v>3900</v>
+      </c>
+      <c r="E26">
+        <v>29.545454545454501</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26">
+        <v>0.5</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="4"/>
+        <v>4.5</v>
+      </c>
+      <c r="J26" s="7">
+        <v>2016</v>
+      </c>
+      <c r="K26" s="7">
+        <f t="shared" si="1"/>
+        <v>33.6</v>
+      </c>
+      <c r="L26" s="7">
+        <v>5916</v>
+      </c>
+      <c r="M26" s="8">
+        <f t="shared" si="2"/>
+        <v>98.6</v>
+      </c>
+      <c r="N26">
+        <v>3900</v>
+      </c>
+      <c r="O26">
+        <v>43.3333333333333</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="3"/>
+        <v>90.000000000000071</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>462</v>
+      </c>
+      <c r="C27">
+        <v>4362</v>
+      </c>
+      <c r="D27">
+        <v>3900</v>
+      </c>
+      <c r="E27">
+        <v>31.707317073170699</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27">
+        <v>2.7</v>
+      </c>
+      <c r="I27">
+        <f>I28+H27</f>
+        <v>4</v>
+      </c>
+      <c r="J27" s="7">
+        <v>2046</v>
+      </c>
+      <c r="K27" s="7">
+        <f t="shared" si="1"/>
+        <v>34.1</v>
+      </c>
+      <c r="L27" s="7">
+        <v>5946</v>
+      </c>
+      <c r="M27" s="8">
+        <f t="shared" si="2"/>
+        <v>99.1</v>
+      </c>
+      <c r="N27">
+        <v>3900</v>
+      </c>
+      <c r="O27">
+        <v>26.351351351351301</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="3"/>
+        <v>148.00000000000028</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>1632</v>
+      </c>
+      <c r="C28">
+        <v>5532</v>
+      </c>
+      <c r="D28">
+        <v>3900</v>
+      </c>
+      <c r="E28">
+        <v>30.46875</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28">
+        <v>1.3</v>
+      </c>
+      <c r="I28">
+        <f>H28</f>
+        <v>1.3</v>
+      </c>
+      <c r="J28" s="10">
+        <v>2208</v>
+      </c>
+      <c r="K28" s="10">
+        <f t="shared" si="1"/>
+        <v>36.799999999999997</v>
+      </c>
+      <c r="L28" s="10">
+        <v>6108</v>
+      </c>
+      <c r="M28" s="11">
+        <f t="shared" si="2"/>
+        <v>101.8</v>
+      </c>
+      <c r="N28">
+        <v>3900</v>
+      </c>
+      <c r="O28">
+        <v>22.807017543859601</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="3"/>
+        <v>171.00000000000037</v>
+      </c>
+      <c r="Q28">
+        <f>SUM(P17:P28)</f>
+        <v>1203.0000000000025</v>
+      </c>
+      <c r="R28" t="s">
+        <v>83</v>
+      </c>
+      <c r="S28">
+        <v>10</v>
+      </c>
+      <c r="U28">
+        <f>Q28/186</f>
+        <v>6.4677419354838843</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>858</v>
+      </c>
+      <c r="C29">
+        <v>4758</v>
+      </c>
+      <c r="D29">
+        <v>3900</v>
+      </c>
+      <c r="E29">
+        <v>18.139534883720899</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29">
+        <v>0.6</v>
+      </c>
+      <c r="I29">
+        <f t="shared" ref="I29:I35" si="5">I30+H29</f>
+        <v>38.099999999999994</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0</v>
+      </c>
+      <c r="K29" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="4">
+        <v>3900</v>
+      </c>
+      <c r="M29" s="5">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="N29">
+        <v>3900</v>
+      </c>
+      <c r="O29">
+        <v>16.25</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <v>1854</v>
+      </c>
+      <c r="C30">
+        <v>5754</v>
+      </c>
+      <c r="D30">
+        <v>3900</v>
+      </c>
+      <c r="E30">
+        <v>55.714285714285701</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="5"/>
+        <v>37.499999999999993</v>
+      </c>
+      <c r="J30" s="7">
+        <v>36</v>
+      </c>
+      <c r="K30" s="7">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+      <c r="L30" s="7">
+        <v>3936</v>
+      </c>
+      <c r="M30" s="8">
+        <f t="shared" si="2"/>
+        <v>65.599999999999994</v>
+      </c>
+      <c r="N30">
+        <v>3900</v>
+      </c>
+      <c r="O30">
+        <v>12.580645161290301</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="3"/>
+        <v>310.00000000000051</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="5"/>
+        <v>35.199999999999996</v>
+      </c>
+      <c r="J31">
+        <v>174</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="1"/>
+        <v>2.9</v>
+      </c>
+      <c r="L31">
+        <v>4434</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="2"/>
+        <v>73.900000000000006</v>
+      </c>
+      <c r="P31">
+        <f>P38/2</f>
+        <v>130.00000000000065</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="G32" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32">
+        <v>6</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="5"/>
+        <v>31.099999999999998</v>
+      </c>
+      <c r="J32">
+        <v>420</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="L32">
+        <v>4884</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="2"/>
+        <v>81.400000000000006</v>
+      </c>
+      <c r="P32">
+        <f>P39/2</f>
+        <v>105.00000000000028</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>1032</v>
+      </c>
+      <c r="C33">
+        <v>4932</v>
+      </c>
+      <c r="D33">
+        <v>3900</v>
+      </c>
+      <c r="E33">
+        <v>15.9183673469387</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="5"/>
+        <v>25.099999999999998</v>
+      </c>
+      <c r="J33" s="7">
+        <v>780</v>
+      </c>
+      <c r="K33" s="7">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="L33" s="7">
+        <v>4680</v>
+      </c>
+      <c r="M33" s="8">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="N33">
+        <v>3900</v>
+      </c>
+      <c r="O33">
+        <v>29.770992366412202</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="3"/>
+        <v>131.00000000000006</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>1236</v>
+      </c>
+      <c r="C34">
+        <v>5136</v>
+      </c>
+      <c r="D34">
+        <v>3900</v>
+      </c>
+      <c r="E34">
+        <v>28.4671532846715</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34">
+        <v>7.1</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="5"/>
+        <v>22.799999999999997</v>
+      </c>
+      <c r="J34" s="7">
+        <v>918</v>
+      </c>
+      <c r="K34" s="7">
+        <f t="shared" si="1"/>
+        <v>15.3</v>
+      </c>
+      <c r="L34" s="7">
+        <v>4818</v>
+      </c>
+      <c r="M34" s="8">
+        <f t="shared" si="2"/>
+        <v>80.3</v>
+      </c>
+      <c r="N34">
+        <v>3900</v>
+      </c>
+      <c r="O34">
+        <v>20.5263157894736</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="3"/>
+        <v>190.0000000000008</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35">
+        <v>1584</v>
+      </c>
+      <c r="C35">
+        <v>5484</v>
+      </c>
+      <c r="D35">
+        <v>3900</v>
+      </c>
+      <c r="E35">
+        <v>29.545454545454501</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H35">
+        <v>4.8</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="5"/>
+        <v>15.7</v>
+      </c>
+      <c r="J35" s="7">
+        <v>1344</v>
+      </c>
+      <c r="K35" s="7">
+        <f t="shared" si="1"/>
+        <v>22.4</v>
+      </c>
+      <c r="L35" s="7">
+        <v>5244</v>
+      </c>
+      <c r="M35" s="8">
+        <f t="shared" si="2"/>
+        <v>87.4</v>
+      </c>
+      <c r="N35">
+        <v>3900</v>
+      </c>
+      <c r="O35">
+        <v>29.545454545454501</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="3"/>
+        <v>132.0000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36">
+        <v>1680</v>
+      </c>
+      <c r="C36">
+        <v>5580</v>
+      </c>
+      <c r="D36">
+        <v>3900</v>
+      </c>
+      <c r="E36">
+        <v>23.780487804878</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H36">
+        <v>3.7</v>
+      </c>
+      <c r="I36">
+        <f>I37+H36</f>
+        <v>10.9</v>
+      </c>
+      <c r="J36" s="7">
+        <v>1632</v>
+      </c>
+      <c r="K36" s="7">
+        <f t="shared" si="1"/>
+        <v>27.2</v>
+      </c>
+      <c r="L36" s="7">
+        <v>5532</v>
+      </c>
+      <c r="M36" s="8">
+        <f t="shared" si="2"/>
+        <v>92.2</v>
+      </c>
+      <c r="N36">
+        <v>3900</v>
+      </c>
+      <c r="O36">
+        <v>30.46875</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="3"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37">
+        <v>1956</v>
+      </c>
+      <c r="C37">
+        <v>5856</v>
+      </c>
+      <c r="D37">
+        <v>3900</v>
+      </c>
+      <c r="E37">
+        <v>31.451612903225801</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H37">
+        <v>7.2</v>
+      </c>
+      <c r="I37">
+        <f>H37</f>
+        <v>7.2</v>
+      </c>
+      <c r="J37" s="10">
+        <v>1854</v>
+      </c>
+      <c r="K37" s="10">
+        <f t="shared" si="1"/>
+        <v>30.9</v>
+      </c>
+      <c r="L37" s="10">
+        <v>5754</v>
+      </c>
+      <c r="M37" s="11">
+        <f t="shared" si="2"/>
+        <v>95.9</v>
+      </c>
+      <c r="N37">
+        <v>3900</v>
+      </c>
+      <c r="O37">
+        <v>55.714285714285701</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="3"/>
+        <v>70.000000000000014</v>
+      </c>
+      <c r="Q37">
+        <f>SUM(P29:P37)</f>
+        <v>1436.0000000000025</v>
+      </c>
+      <c r="R37" t="s">
+        <v>83</v>
+      </c>
+      <c r="S37">
+        <v>30</v>
+      </c>
+      <c r="U37">
+        <f>Q37/186</f>
+        <v>7.7204301075268953</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <v>2160</v>
+      </c>
+      <c r="C38">
+        <v>6060</v>
+      </c>
+      <c r="D38">
+        <v>3900</v>
+      </c>
+      <c r="E38">
+        <v>18.309859154929502</v>
+      </c>
+      <c r="G38" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38">
+        <v>174</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="1"/>
+        <v>2.9</v>
+      </c>
+      <c r="L38">
+        <v>4434</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="2"/>
+        <v>73.900000000000006</v>
+      </c>
+      <c r="N38">
+        <v>4260</v>
+      </c>
+      <c r="O38">
+        <v>16.384615384615302</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="3"/>
+        <v>260.00000000000131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39">
+        <v>2232</v>
+      </c>
+      <c r="C39">
+        <v>6132</v>
+      </c>
+      <c r="D39">
+        <v>3900</v>
+      </c>
+      <c r="E39">
+        <v>21.081081081080999</v>
+      </c>
+      <c r="G39" t="s">
+        <v>24</v>
+      </c>
+      <c r="J39">
+        <v>420</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="L39">
+        <v>4884</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="2"/>
+        <v>81.400000000000006</v>
+      </c>
+      <c r="N39">
+        <v>4464</v>
+      </c>
+      <c r="O39">
+        <v>21.257142857142799</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="3"/>
+        <v>210.00000000000057</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40">
+        <v>324</v>
+      </c>
+      <c r="C40">
+        <v>4224</v>
+      </c>
+      <c r="D40">
+        <v>3900</v>
+      </c>
+      <c r="E40">
+        <v>49.367088607594901</v>
+      </c>
+      <c r="G40" t="s">
+        <v>11</v>
+      </c>
+      <c r="J40">
+        <v>1344</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="1"/>
+        <v>22.4</v>
+      </c>
+      <c r="L40">
+        <v>5298</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="2"/>
+        <v>88.3</v>
+      </c>
+      <c r="N40">
+        <v>3954</v>
+      </c>
+      <c r="O40">
+        <v>17.972727272727202</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="3"/>
+        <v>220.00000000000088</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>3</v>
+      </c>
+      <c r="L42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J43">
+        <v>6</v>
+      </c>
+      <c r="L43">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="J44">
+        <v>3906</v>
+      </c>
+      <c r="L44">
+        <v>4098</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G3:O40">
+    <sortCondition ref="G1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E112AF5-6125-4347-8F9A-6D7F040BBD30}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
generovanie rieseni okoli. Vozidlo check vkladania vyberania na debug, model upraveny
</commit_message>
<xml_diff>
--- a/Generovanie kodu.xlsx
+++ b/Generovanie kodu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrej Beliančin\Projects\DIS-SEM-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrejbeliancin/Desktop/GIT/DIS-SEM-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA5BF2D-BE1A-4A1F-B2FF-BBC8962A3566}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E74D34-0EB3-0B47-A0C0-CCA0ED5D5A49}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CAA8F1F5-8409-4114-88BB-3627D0CE125A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{CAA8F1F5-8409-4114-88BB-3627D0CE125A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="82">
   <si>
     <t>Linka A</t>
   </si>
@@ -266,18 +266,6 @@
     <t>Zaciatok zapasu</t>
   </si>
   <si>
-    <t>Súčet</t>
-  </si>
-  <si>
-    <t>Priemer</t>
-  </si>
-  <si>
-    <t>Medzisúčet</t>
-  </si>
-  <si>
-    <t>Počet</t>
-  </si>
-  <si>
     <t>Pocet zakaznikov</t>
   </si>
   <si>
@@ -288,6 +276,9 @@
   </si>
   <si>
     <t>doba jazdy k stadionu</t>
+  </si>
+  <si>
+    <t>kedy moze posledny autobus prist</t>
   </si>
 </sst>
 </file>
@@ -419,7 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -435,7 +426,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív balíka Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -737,20 +728,20 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="10" max="10" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -770,7 +761,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -800,7 +791,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -830,7 +821,7 @@
         <v>2088</v>
       </c>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -860,7 +851,7 @@
         <v>1950</v>
       </c>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -890,7 +881,7 @@
         <v>1824</v>
       </c>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -916,7 +907,7 @@
         <v>1752</v>
       </c>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -946,7 +937,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -976,7 +967,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -1006,7 +997,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -1032,7 +1023,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -1062,7 +1053,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -1092,7 +1083,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>14</v>
       </c>
@@ -1122,7 +1113,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>15</v>
       </c>
@@ -1152,7 +1143,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>16</v>
       </c>
@@ -1179,7 +1170,7 @@
       </c>
       <c r="T16" s="2"/>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>40</v>
       </c>
@@ -1198,21 +1189,21 @@
       </c>
       <c r="T17" s="2"/>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="1"/>
       <c r="T18" s="2"/>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="1"/>
       <c r="T19" s="2"/>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>1</v>
       </c>
@@ -1225,7 +1216,7 @@
       </c>
       <c r="T20" s="2"/>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>20</v>
       </c>
@@ -1247,7 +1238,7 @@
         <v>new ZastavkaLinky(zastavky.get("BA"), 1.2 * 60.0, zastavky.get("BB")),</v>
       </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -1269,7 +1260,7 @@
         <v>new ZastavkaLinky(zastavky.get("BB"), 2.3 * 60.0, zastavky.get("BC")),</v>
       </c>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -1294,7 +1285,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -1319,7 +1310,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>24</v>
       </c>
@@ -1340,7 +1331,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>25</v>
       </c>
@@ -1365,7 +1356,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -1387,7 +1378,7 @@
         <v>new ZastavkaLinky(zastavky.get("BF"), 3 * 60.0, zastavky.get("K3")),</v>
       </c>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>11</v>
       </c>
@@ -1405,7 +1396,7 @@
         <v>new ZastavkaLinky(zastavky.get("K3"), 6 * 60.0, zastavky.get("BG")),</v>
       </c>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>27</v>
       </c>
@@ -1427,7 +1418,7 @@
         <v>new ZastavkaLinky(zastavky.get("BG"), 4.3 * 60.0, zastavky.get("BH")),</v>
       </c>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>28</v>
       </c>
@@ -1449,7 +1440,7 @@
         <v>new ZastavkaLinky(zastavky.get("BH"), 0.5 * 60.0, zastavky.get("BI")),</v>
       </c>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>29</v>
       </c>
@@ -1471,7 +1462,7 @@
         <v>new ZastavkaLinky(zastavky.get("BI"), 2.7 * 60.0, zastavky.get("BJ")),</v>
       </c>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>30</v>
       </c>
@@ -1493,7 +1484,7 @@
         <v>new ZastavkaLinky(zastavky.get("BJ"), 1.3 * 60.0, zastavky.get("ST"))</v>
       </c>
     </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>40</v>
       </c>
@@ -1511,19 +1502,19 @@
         <v>new ZastavkaLinky(zastavky.get("ST"), 10 * 60.0, zastavky.get("BA"))</v>
       </c>
     </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>20</v>
       </c>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>19</v>
       </c>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>1</v>
       </c>
@@ -1535,7 +1526,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>31</v>
       </c>
@@ -1561,7 +1552,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>32</v>
       </c>
@@ -1587,7 +1578,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>7</v>
       </c>
@@ -1609,7 +1600,7 @@
         <v>245.99999999999997</v>
       </c>
     </row>
-    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>24</v>
       </c>
@@ -1631,7 +1622,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>33</v>
       </c>
@@ -1657,7 +1648,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>34</v>
       </c>
@@ -1683,7 +1674,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="43" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>35</v>
       </c>
@@ -1709,7 +1700,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>36</v>
       </c>
@@ -1735,7 +1726,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="45" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>37</v>
       </c>
@@ -1761,7 +1752,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="46" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>40</v>
       </c>
@@ -1780,7 +1771,7 @@
         <v>2286</v>
       </c>
     </row>
-    <row r="47" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>31</v>
       </c>
@@ -1794,31 +1785,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C15344-21F8-4E67-A098-0EABFA05ED44}">
-  <dimension ref="A1:U44"/>
+  <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" sqref="G14:G15"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="111" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="7" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" customWidth="1"/>
-    <col min="12" max="12" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.42578125" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.5" customWidth="1"/>
+    <col min="14" max="14" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -1834,7 +1826,7 @@
         <v>1.885</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1854,10 +1846,10 @@
         <v>69</v>
       </c>
       <c r="H2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J2" t="s">
         <v>74</v>
@@ -1872,10 +1864,10 @@
         <v>73</v>
       </c>
       <c r="P2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1926,7 +1918,7 @@
         <v>123.00000000000013</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1977,7 +1969,7 @@
         <v>92.000000000000185</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2028,7 +2020,7 @@
         <v>241.00000000000122</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2079,7 +2071,7 @@
         <v>123.00000000000013</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="G7" s="6" t="s">
         <v>7</v>
       </c>
@@ -2109,7 +2101,7 @@
         <v>130.00000000000065</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2160,7 +2152,7 @@
         <v>215.00000000000037</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2211,7 +2203,7 @@
         <v>245.00000000000117</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2262,7 +2254,7 @@
         <v>137.00000000000017</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="G11" s="6" t="s">
         <v>11</v>
       </c>
@@ -2292,7 +2284,7 @@
         <v>110.00000000000044</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2343,7 +2335,7 @@
         <v>132.0000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -2394,7 +2386,7 @@
         <v>164.00000000000034</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2445,7 +2437,7 @@
         <v>124.00000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -2496,7 +2488,7 @@
         <v>213.00000000000088</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -2551,7 +2543,7 @@
         <v>2234.0000000000068</v>
       </c>
       <c r="R16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="S16">
         <v>25</v>
@@ -2560,8 +2552,15 @@
         <f>Q16/186</f>
         <v>12.010752688172079</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V16" t="s">
+        <v>81</v>
+      </c>
+      <c r="W16">
+        <f>L16-(I3*60)</f>
+        <v>3852.0000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -2612,7 +2611,7 @@
         <v>79.000000000000057</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2663,7 +2662,7 @@
         <v>69.000000000000099</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -2714,7 +2713,7 @@
         <v>43.000000000000021</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2765,7 +2764,7 @@
         <v>127.00000000000014</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="G21" s="6" t="s">
         <v>24</v>
       </c>
@@ -2795,7 +2794,7 @@
         <v>105.00000000000028</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -2846,7 +2845,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2897,7 +2896,7 @@
         <v>69.000000000000099</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="G24" s="6" t="s">
         <v>11</v>
       </c>
@@ -2927,7 +2926,7 @@
         <v>110.00000000000044</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -2978,7 +2977,7 @@
         <v>162.00000000000048</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -3029,7 +3028,7 @@
         <v>90.000000000000071</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -3080,7 +3079,7 @@
         <v>148.00000000000028</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -3135,7 +3134,7 @@
         <v>1203.0000000000025</v>
       </c>
       <c r="R28" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="S28">
         <v>10</v>
@@ -3144,8 +3143,15 @@
         <f>Q28/186</f>
         <v>6.4677419354838843</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V28" t="s">
+        <v>81</v>
+      </c>
+      <c r="W28">
+        <f>L28-(I17*60)</f>
+        <v>4146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -3196,7 +3202,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -3247,7 +3253,7 @@
         <v>310.00000000000051</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="G31" s="6" t="s">
         <v>7</v>
       </c>
@@ -3277,7 +3283,7 @@
         <v>130.00000000000065</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="G32" s="6" t="s">
         <v>24</v>
       </c>
@@ -3307,7 +3313,7 @@
         <v>105.00000000000028</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -3358,7 +3364,7 @@
         <v>131.00000000000006</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -3409,7 +3415,7 @@
         <v>190.0000000000008</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -3460,7 +3466,7 @@
         <v>132.0000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -3511,7 +3517,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -3566,7 +3572,7 @@
         <v>1436.0000000000025</v>
       </c>
       <c r="R37" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="S37">
         <v>30</v>
@@ -3575,8 +3581,15 @@
         <f>Q37/186</f>
         <v>7.7204301075268953</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V37" t="s">
+        <v>81</v>
+      </c>
+      <c r="W37">
+        <f>L37-(I29*60)</f>
+        <v>3468.0000000000005</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -3620,7 +3633,7 @@
         <v>260.00000000000131</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -3664,7 +3677,7 @@
         <v>210.00000000000057</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -3708,7 +3721,7 @@
         <v>220.00000000000088</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="J42" t="s">
         <v>3</v>
       </c>
@@ -3716,7 +3729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="J43">
         <v>6</v>
       </c>
@@ -3724,7 +3737,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="J44">
         <v>3906</v>
       </c>
@@ -3737,6 +3750,7 @@
     <sortCondition ref="G1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3746,7 +3760,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix proces natup cestujuceho
</commit_message>
<xml_diff>
--- a/Generovanie kodu.xlsx
+++ b/Generovanie kodu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrej Beliančin\Projects\DIS-SEM-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75ED5EB7-3858-4FC4-9F74-1DF9B2746CD0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4059B440-8BEF-4DC1-AEAB-04818809CDF8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CAA8F1F5-8409-4114-88BB-3627D0CE125A}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
     <sheet name="Hárok2" sheetId="2" r:id="rId2"/>
     <sheet name="Hárok3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hárok4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="90">
   <si>
     <t>Linka A</t>
   </si>
@@ -279,14 +280,50 @@
   </si>
   <si>
     <t>kedy moze posledny autobus prist</t>
+  </si>
+  <si>
+    <t>Doba jazdy k štadiónu</t>
+  </si>
+  <si>
+    <t>Čas príchodu prvého zákazníka</t>
+  </si>
+  <si>
+    <t>Čas príchodu posledného zákazníka</t>
+  </si>
+  <si>
+    <t>Dĺžka intervalu</t>
+  </si>
+  <si>
+    <t>Parameter exponeniálneho rozdelenia(stredná hodnota)</t>
+  </si>
+  <si>
+    <t>Maximálny počet zákazníkov</t>
+  </si>
+  <si>
+    <t>Maximálny počet cestujúcich na zastávke</t>
+  </si>
+  <si>
+    <t>Linka A 2 krat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -303,7 +340,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -391,11 +428,146 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -408,6 +580,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -724,7 +924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD79F5DF-5EE7-4CA7-B719-F55D9FC90063}">
   <dimension ref="B1:U47"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -1785,10 +1985,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C15344-21F8-4E67-A098-0EABFA05ED44}">
-  <dimension ref="A1:W44"/>
+  <dimension ref="A1:X49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W35" sqref="W35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,6 +1998,7 @@
     <col min="3" max="3" width="24.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="15" customWidth="1"/>
     <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27" bestFit="1" customWidth="1"/>
@@ -1808,14 +2009,19 @@
     <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="27" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>76</v>
       </c>
       <c r="B1">
         <v>6786</v>
+      </c>
+      <c r="C1" s="12">
+        <f>B1/86400</f>
+        <v>7.8541666666666662E-2</v>
       </c>
       <c r="M1">
         <f>B1/60</f>
@@ -1826,7 +2032,7 @@
         <v>1.885</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -1867,7 +2073,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1882,6 +2088,10 @@
       </c>
       <c r="E3">
         <v>56.521739130434703</v>
+      </c>
+      <c r="F3" s="12">
+        <f>J3/86400</f>
+        <v>6.9444444444444444E-5</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>3</v>
@@ -1918,7 +2128,7 @@
         <v>123.00000000000013</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1933,6 +2143,10 @@
       </c>
       <c r="E4">
         <v>90.697674418604606</v>
+      </c>
+      <c r="F4" s="12">
+        <f>J4/86400</f>
+        <v>2.2916666666666667E-3</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>4</v>
@@ -1969,7 +2183,7 @@
         <v>92.000000000000185</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1984,6 +2198,10 @@
       </c>
       <c r="E5">
         <v>30.708661417322801</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" ref="F5:F40" si="4">J5/86400</f>
+        <v>3.8888888888888888E-3</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>5</v>
@@ -2020,7 +2238,7 @@
         <v>241.00000000000122</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2035,6 +2253,10 @@
       </c>
       <c r="E6">
         <v>130</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" si="4"/>
+        <v>5.347222222222222E-3</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>6</v>
@@ -2071,7 +2293,11 @@
         <v>123.00000000000013</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F7" s="12">
+        <f t="shared" si="4"/>
+        <v>2.0138888888888888E-3</v>
+      </c>
       <c r="G7" s="6" t="s">
         <v>7</v>
       </c>
@@ -2101,7 +2327,7 @@
         <v>130.00000000000065</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2116,6 +2342,10 @@
       </c>
       <c r="E8">
         <v>56.521739130434703</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" si="4"/>
+        <v>9.9305555555555553E-3</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>8</v>
@@ -2152,7 +2382,7 @@
         <v>215.00000000000037</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2167,6 +2397,10 @@
       </c>
       <c r="E9">
         <v>24.074074074074002</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" si="4"/>
+        <v>1.1944444444444445E-2</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>9</v>
@@ -2203,7 +2437,7 @@
         <v>245.00000000000117</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2218,6 +2452,10 @@
       </c>
       <c r="E10">
         <v>43.3333333333333</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="4"/>
+        <v>1.4305555555555556E-2</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>10</v>
@@ -2254,7 +2492,11 @@
         <v>137.00000000000017</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F11" s="12">
+        <f t="shared" si="4"/>
+        <v>1.5555555555555555E-2</v>
+      </c>
       <c r="G11" s="6" t="s">
         <v>11</v>
       </c>
@@ -2284,7 +2526,7 @@
         <v>110.00000000000044</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2299,6 +2541,10 @@
       </c>
       <c r="E12">
         <v>16.384615384615302</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="4"/>
+        <v>1.8333333333333333E-2</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>12</v>
@@ -2335,7 +2581,7 @@
         <v>132.0000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -2350,6 +2596,10 @@
       </c>
       <c r="E13">
         <v>26.351351351351301</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="4"/>
+        <v>1.9444444444444445E-2</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>13</v>
@@ -2386,7 +2636,7 @@
         <v>164.00000000000034</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2401,6 +2651,10 @@
       </c>
       <c r="E14">
         <v>21.257142857142799</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="4"/>
+        <v>2.2638888888888889E-2</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>14</v>
@@ -2437,7 +2691,7 @@
         <v>124.00000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -2452,6 +2706,10 @@
       </c>
       <c r="E15">
         <v>22.807017543859601</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="4"/>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>15</v>
@@ -2488,7 +2746,7 @@
         <v>213.00000000000088</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -2503,6 +2761,10 @@
       </c>
       <c r="E16">
         <v>17.972727272727202</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" si="4"/>
+        <v>2.5833333333333333E-2</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>16</v>
@@ -2559,8 +2821,12 @@
         <f>L16-(I3*60)</f>
         <v>3852.0000000000005</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X16" s="12">
+        <f>W16/86400</f>
+        <v>4.4583333333333336E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -2576,6 +2842,10 @@
       <c r="E17">
         <v>16.25</v>
       </c>
+      <c r="F17" s="12">
+        <f t="shared" si="4"/>
+        <v>3.7499999999999999E-3</v>
+      </c>
       <c r="G17" s="3" t="s">
         <v>20</v>
       </c>
@@ -2583,7 +2853,7 @@
         <v>1.2</v>
       </c>
       <c r="I17">
-        <f t="shared" ref="I17:I26" si="4">I18+H17</f>
+        <f t="shared" ref="I17:I26" si="5">I18+H17</f>
         <v>32.700000000000003</v>
       </c>
       <c r="J17" s="4">
@@ -2611,7 +2881,7 @@
         <v>79.000000000000057</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2627,6 +2897,10 @@
       <c r="E18">
         <v>12.580645161290301</v>
       </c>
+      <c r="F18" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5833333333333334E-3</v>
+      </c>
       <c r="G18" s="6" t="s">
         <v>21</v>
       </c>
@@ -2634,7 +2908,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>31.5</v>
       </c>
       <c r="J18" s="7">
@@ -2662,7 +2936,7 @@
         <v>69.000000000000099</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -2678,6 +2952,10 @@
       <c r="E19">
         <v>31.707317073170699</v>
       </c>
+      <c r="F19" s="12">
+        <f t="shared" si="4"/>
+        <v>6.1805555555555555E-3</v>
+      </c>
       <c r="G19" s="6" t="s">
         <v>22</v>
       </c>
@@ -2685,7 +2963,7 @@
         <v>3.2</v>
       </c>
       <c r="I19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>29.2</v>
       </c>
       <c r="J19" s="7">
@@ -2713,7 +2991,7 @@
         <v>43.000000000000021</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2729,6 +3007,10 @@
       <c r="E20">
         <v>29.770992366412202</v>
       </c>
+      <c r="F20" s="12">
+        <f t="shared" si="4"/>
+        <v>8.4027777777777781E-3</v>
+      </c>
       <c r="G20" s="6" t="s">
         <v>23</v>
       </c>
@@ -2736,7 +3018,7 @@
         <v>4.3</v>
       </c>
       <c r="I20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="J20" s="7">
@@ -2764,7 +3046,11 @@
         <v>127.00000000000014</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F21" s="12">
+        <f t="shared" si="4"/>
+        <v>4.8611111111111112E-3</v>
+      </c>
       <c r="G21" s="6" t="s">
         <v>24</v>
       </c>
@@ -2772,7 +3058,7 @@
         <v>1.2</v>
       </c>
       <c r="I21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>21.7</v>
       </c>
       <c r="J21">
@@ -2794,7 +3080,7 @@
         <v>105.00000000000028</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -2810,6 +3096,10 @@
       <c r="E22">
         <v>42.391304347826001</v>
       </c>
+      <c r="F22" s="12">
+        <f t="shared" si="4"/>
+        <v>1.2222222222222223E-2</v>
+      </c>
       <c r="G22" s="6" t="s">
         <v>25</v>
       </c>
@@ -2817,7 +3107,7 @@
         <v>2.7</v>
       </c>
       <c r="I22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20.5</v>
       </c>
       <c r="J22" s="7">
@@ -2845,7 +3135,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -2861,6 +3151,10 @@
       <c r="E23">
         <v>20.5263157894736</v>
       </c>
+      <c r="F23" s="12">
+        <f t="shared" si="4"/>
+        <v>1.4097222222222223E-2</v>
+      </c>
       <c r="G23" s="6" t="s">
         <v>26</v>
       </c>
@@ -2868,7 +3162,7 @@
         <v>3</v>
       </c>
       <c r="I23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.8</v>
       </c>
       <c r="J23" s="7">
@@ -2896,7 +3190,11 @@
         <v>69.000000000000099</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F24" s="12">
+        <f t="shared" si="4"/>
+        <v>1.5555555555555555E-2</v>
+      </c>
       <c r="G24" s="6" t="s">
         <v>11</v>
       </c>
@@ -2904,7 +3202,7 @@
         <v>6</v>
       </c>
       <c r="I24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14.8</v>
       </c>
       <c r="J24">
@@ -2926,7 +3224,7 @@
         <v>110.00000000000044</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -2942,6 +3240,10 @@
       <c r="E25">
         <v>16.182572614107801</v>
       </c>
+      <c r="F25" s="12">
+        <f t="shared" si="4"/>
+        <v>2.0347222222222221E-2</v>
+      </c>
       <c r="G25" s="6" t="s">
         <v>27</v>
       </c>
@@ -2949,7 +3251,7 @@
         <v>4.3</v>
       </c>
       <c r="I25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.8000000000000007</v>
       </c>
       <c r="J25" s="7">
@@ -2977,7 +3279,7 @@
         <v>162.00000000000048</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -2993,6 +3295,10 @@
       <c r="E26">
         <v>29.545454545454501</v>
       </c>
+      <c r="F26" s="12">
+        <f t="shared" si="4"/>
+        <v>2.3333333333333334E-2</v>
+      </c>
       <c r="G26" s="6" t="s">
         <v>28</v>
       </c>
@@ -3000,7 +3306,7 @@
         <v>0.5</v>
       </c>
       <c r="I26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.5</v>
       </c>
       <c r="J26" s="7">
@@ -3028,7 +3334,7 @@
         <v>90.000000000000071</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -3043,6 +3349,10 @@
       </c>
       <c r="E27">
         <v>31.707317073170699</v>
+      </c>
+      <c r="F27" s="12">
+        <f t="shared" si="4"/>
+        <v>2.3680555555555555E-2</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>29</v>
@@ -3079,7 +3389,7 @@
         <v>148.00000000000028</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -3094,6 +3404,10 @@
       </c>
       <c r="E28">
         <v>30.46875</v>
+      </c>
+      <c r="F28" s="12">
+        <f t="shared" si="4"/>
+        <v>2.5555555555555557E-2</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>30</v>
@@ -3150,8 +3464,12 @@
         <f>L28-(I17*60)</f>
         <v>4146</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X28" s="12">
+        <f>W28/86400</f>
+        <v>4.7986111111111111E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -3167,6 +3485,10 @@
       <c r="E29">
         <v>18.139534883720899</v>
       </c>
+      <c r="F29" s="12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="G29" s="3" t="s">
         <v>31</v>
       </c>
@@ -3174,7 +3496,7 @@
         <v>0.6</v>
       </c>
       <c r="I29">
-        <f t="shared" ref="I29:I35" si="5">I30+H29</f>
+        <f t="shared" ref="I29:I35" si="6">I30+H29</f>
         <v>38.099999999999994</v>
       </c>
       <c r="J29" s="4">
@@ -3202,7 +3524,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -3218,6 +3540,10 @@
       <c r="E30">
         <v>55.714285714285701</v>
       </c>
+      <c r="F30" s="12">
+        <f t="shared" si="4"/>
+        <v>4.1666666666666669E-4</v>
+      </c>
       <c r="G30" s="6" t="s">
         <v>32</v>
       </c>
@@ -3225,7 +3551,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>37.499999999999993</v>
       </c>
       <c r="J30" s="7">
@@ -3253,7 +3579,11 @@
         <v>310.00000000000051</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F31" s="12">
+        <f t="shared" si="4"/>
+        <v>2.0138888888888888E-3</v>
+      </c>
       <c r="G31" s="6" t="s">
         <v>7</v>
       </c>
@@ -3261,7 +3591,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="I31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>35.199999999999996</v>
       </c>
       <c r="J31">
@@ -3283,7 +3613,11 @@
         <v>130.00000000000065</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="F32" s="12">
+        <f t="shared" si="4"/>
+        <v>4.8611111111111112E-3</v>
+      </c>
       <c r="G32" s="6" t="s">
         <v>24</v>
       </c>
@@ -3291,7 +3625,7 @@
         <v>6</v>
       </c>
       <c r="I32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>31.099999999999998</v>
       </c>
       <c r="J32">
@@ -3313,7 +3647,7 @@
         <v>105.00000000000028</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -3329,6 +3663,10 @@
       <c r="E33">
         <v>15.9183673469387</v>
       </c>
+      <c r="F33" s="12">
+        <f t="shared" si="4"/>
+        <v>9.0277777777777769E-3</v>
+      </c>
       <c r="G33" s="6" t="s">
         <v>33</v>
       </c>
@@ -3336,7 +3674,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>25.099999999999998</v>
       </c>
       <c r="J33" s="7">
@@ -3364,7 +3702,7 @@
         <v>131.00000000000006</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -3380,6 +3718,10 @@
       <c r="E34">
         <v>28.4671532846715</v>
       </c>
+      <c r="F34" s="12">
+        <f t="shared" si="4"/>
+        <v>1.0625000000000001E-2</v>
+      </c>
       <c r="G34" s="6" t="s">
         <v>34</v>
       </c>
@@ -3387,7 +3729,7 @@
         <v>7.1</v>
       </c>
       <c r="I34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22.799999999999997</v>
       </c>
       <c r="J34" s="7">
@@ -3415,7 +3757,7 @@
         <v>190.0000000000008</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -3431,6 +3773,10 @@
       <c r="E35">
         <v>29.545454545454501</v>
       </c>
+      <c r="F35" s="12">
+        <f t="shared" si="4"/>
+        <v>1.5555555555555555E-2</v>
+      </c>
       <c r="G35" s="6" t="s">
         <v>35</v>
       </c>
@@ -3438,7 +3784,7 @@
         <v>4.8</v>
       </c>
       <c r="I35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15.7</v>
       </c>
       <c r="J35" s="7">
@@ -3466,7 +3812,7 @@
         <v>132.0000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -3481,6 +3827,10 @@
       </c>
       <c r="E36">
         <v>23.780487804878</v>
+      </c>
+      <c r="F36" s="12">
+        <f t="shared" si="4"/>
+        <v>1.8888888888888889E-2</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>36</v>
@@ -3517,7 +3867,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -3532,6 +3882,10 @@
       </c>
       <c r="E37">
         <v>31.451612903225801</v>
+      </c>
+      <c r="F37" s="12">
+        <f t="shared" si="4"/>
+        <v>2.1458333333333333E-2</v>
       </c>
       <c r="G37" s="9" t="s">
         <v>37</v>
@@ -3588,8 +3942,12 @@
         <f>L37-(I29*60)</f>
         <v>3468.0000000000005</v>
       </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X37" s="12">
+        <f>W37/86400</f>
+        <v>4.0138888888888898E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>15</v>
       </c>
@@ -3604,6 +3962,10 @@
       </c>
       <c r="E38">
         <v>18.309859154929502</v>
+      </c>
+      <c r="F38" s="12">
+        <f t="shared" si="4"/>
+        <v>2.0138888888888888E-3</v>
       </c>
       <c r="G38" t="s">
         <v>7</v>
@@ -3633,7 +3995,7 @@
         <v>260.00000000000131</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -3648,6 +4010,10 @@
       </c>
       <c r="E39">
         <v>21.081081081080999</v>
+      </c>
+      <c r="F39" s="12">
+        <f t="shared" si="4"/>
+        <v>4.8611111111111112E-3</v>
       </c>
       <c r="G39" t="s">
         <v>24</v>
@@ -3677,7 +4043,7 @@
         <v>210.00000000000057</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -3692,6 +4058,10 @@
       </c>
       <c r="E40">
         <v>49.367088607594901</v>
+      </c>
+      <c r="F40" s="12">
+        <f t="shared" si="4"/>
+        <v>1.5555555555555555E-2</v>
       </c>
       <c r="G40" t="s">
         <v>11</v>
@@ -3721,7 +4091,7 @@
         <v>220.00000000000088</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="J42" t="s">
         <v>3</v>
       </c>
@@ -3729,7 +4099,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="J43">
         <v>6</v>
       </c>
@@ -3737,12 +4107,54 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="J44">
         <v>3906</v>
       </c>
       <c r="L44">
         <v>4098</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>89</v>
+      </c>
+      <c r="H45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <f>SUM(H45:H47)</f>
+        <v>101</v>
+      </c>
+      <c r="I48" s="12">
+        <f>H48/(86400 / 60)</f>
+        <v>7.013888888888889E-2</v>
+      </c>
+      <c r="J48" s="12">
+        <f>H47/(86400 / 60)</f>
+        <v>2.6388888888888889E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I49" s="12">
+        <f>$C$1-I48</f>
+        <v>8.4027777777777729E-3</v>
+      </c>
+      <c r="J49" s="12">
+        <f>$C$1-J48</f>
+        <v>5.215277777777777E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3756,12 +4168,2881 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E112AF5-6125-4347-8F9A-6D7F040BBD30}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:U40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:O16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" customWidth="1"/>
+    <col min="12" max="12" width="5.140625" customWidth="1"/>
+    <col min="13" max="13" width="3.7109375" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
+    <col min="15" max="15" width="27.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C1">
+        <v>86400</v>
+      </c>
+      <c r="D1">
+        <f>60*60*24</f>
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N2" t="s">
+        <v>86</v>
+      </c>
+      <c r="O2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="12">
+        <f>E3/(86400/60)</f>
+        <v>2.6388888888888885E-2</v>
+      </c>
+      <c r="D3">
+        <v>3.2</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E13" si="0">E4+D3</f>
+        <v>37.999999999999993</v>
+      </c>
+      <c r="F3" s="12">
+        <f>I3/$C$1</f>
+        <v>6.9444444444444444E-5</v>
+      </c>
+      <c r="G3" s="12">
+        <f>K3/$C$1</f>
+        <v>4.5208333333333336E-2</v>
+      </c>
+      <c r="H3" s="12">
+        <f>G3-F3</f>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <f>I3/60</f>
+        <v>0.1</v>
+      </c>
+      <c r="K3">
+        <v>3906</v>
+      </c>
+      <c r="L3">
+        <f>K3/60</f>
+        <v>65.099999999999994</v>
+      </c>
+      <c r="M3">
+        <v>3900</v>
+      </c>
+      <c r="N3">
+        <v>31.707317073170699</v>
+      </c>
+      <c r="O3">
+        <f>M3/N3</f>
+        <v>123.00000000000013</v>
+      </c>
+      <c r="S3" s="12">
+        <f>U3/(86400/60)</f>
+        <v>7.8541666666666662E-2</v>
+      </c>
+      <c r="U3">
+        <v>113.1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="12">
+        <f t="shared" ref="C4:C37" si="1">E4/(86400/60)</f>
+        <v>2.4166666666666659E-2</v>
+      </c>
+      <c r="D4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>34.79999999999999</v>
+      </c>
+      <c r="F4" s="12">
+        <f t="shared" ref="F4:F40" si="2">I4/$C$1</f>
+        <v>2.2916666666666667E-3</v>
+      </c>
+      <c r="G4" s="12">
+        <f t="shared" ref="G4:G40" si="3">K4/$C$1</f>
+        <v>4.7430555555555552E-2</v>
+      </c>
+      <c r="H4" s="12">
+        <f t="shared" ref="H4:H40" si="4">G4-F4</f>
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="I4">
+        <v>198</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J40" si="5">I4/60</f>
+        <v>3.3</v>
+      </c>
+      <c r="K4">
+        <v>4098</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L40" si="6">K4/60</f>
+        <v>68.3</v>
+      </c>
+      <c r="M4">
+        <v>3900</v>
+      </c>
+      <c r="N4">
+        <v>42.391304347826001</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O40" si="7">M4/N4</f>
+        <v>92.000000000000185</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="12">
+        <f t="shared" si="1"/>
+        <v>2.2569444444444441E-2</v>
+      </c>
+      <c r="D5">
+        <v>2.1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>32.499999999999993</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" si="2"/>
+        <v>3.8888888888888888E-3</v>
+      </c>
+      <c r="G5" s="12">
+        <f t="shared" si="3"/>
+        <v>4.9027777777777781E-2</v>
+      </c>
+      <c r="H5" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="I5">
+        <v>336</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="5"/>
+        <v>5.6</v>
+      </c>
+      <c r="K5">
+        <v>4236</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="6"/>
+        <v>70.599999999999994</v>
+      </c>
+      <c r="M5">
+        <v>3900</v>
+      </c>
+      <c r="N5">
+        <v>16.182572614107801</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="7"/>
+        <v>241.00000000000122</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="12">
+        <f t="shared" si="1"/>
+        <v>2.1111111111111108E-2</v>
+      </c>
+      <c r="D6">
+        <v>1.2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>30.399999999999995</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" si="2"/>
+        <v>5.347222222222222E-3</v>
+      </c>
+      <c r="G6" s="12">
+        <f t="shared" si="3"/>
+        <v>5.0486111111111114E-2</v>
+      </c>
+      <c r="H6" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="I6">
+        <v>462</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="5"/>
+        <v>7.7</v>
+      </c>
+      <c r="K6">
+        <v>4362</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="6"/>
+        <v>72.7</v>
+      </c>
+      <c r="M6">
+        <v>3900</v>
+      </c>
+      <c r="N6">
+        <v>31.707317073170699</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="7"/>
+        <v>123.00000000000013</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="12">
+        <f t="shared" si="1"/>
+        <v>2.0277777777777777E-2</v>
+      </c>
+      <c r="D7">
+        <v>5.4</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>29.199999999999996</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="O7">
+        <f>O38/2</f>
+        <v>130.00000000000065</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="12">
+        <f t="shared" si="1"/>
+        <v>1.6527777777777777E-2</v>
+      </c>
+      <c r="D8">
+        <v>2.9</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>23.799999999999997</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" si="2"/>
+        <v>9.9305555555555553E-3</v>
+      </c>
+      <c r="G8" s="12">
+        <f t="shared" si="3"/>
+        <v>5.5069444444444442E-2</v>
+      </c>
+      <c r="H8" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="I8">
+        <v>858</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="5"/>
+        <v>14.3</v>
+      </c>
+      <c r="K8">
+        <v>4758</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="6"/>
+        <v>79.3</v>
+      </c>
+      <c r="M8">
+        <v>3900</v>
+      </c>
+      <c r="N8">
+        <v>18.139534883720899</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="7"/>
+        <v>215.00000000000037</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="12">
+        <f t="shared" si="1"/>
+        <v>1.4513888888888889E-2</v>
+      </c>
+      <c r="D9">
+        <v>3.4</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>20.9</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" si="2"/>
+        <v>1.1944444444444445E-2</v>
+      </c>
+      <c r="G9" s="12">
+        <f t="shared" si="3"/>
+        <v>5.7083333333333333E-2</v>
+      </c>
+      <c r="H9" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="I9">
+        <v>1032</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="5"/>
+        <v>17.2</v>
+      </c>
+      <c r="K9">
+        <v>4932</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="6"/>
+        <v>82.2</v>
+      </c>
+      <c r="M9">
+        <v>3900</v>
+      </c>
+      <c r="N9">
+        <v>15.9183673469387</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="7"/>
+        <v>245.00000000000117</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="12">
+        <f t="shared" si="1"/>
+        <v>1.2152777777777778E-2</v>
+      </c>
+      <c r="D10">
+        <v>1.8</v>
+      </c>
+      <c r="E10">
+        <f>E11+D10</f>
+        <v>17.5</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="2"/>
+        <v>1.4305555555555556E-2</v>
+      </c>
+      <c r="G10" s="12">
+        <f t="shared" si="3"/>
+        <v>5.9444444444444446E-2</v>
+      </c>
+      <c r="H10" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="I10">
+        <v>1236</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="5"/>
+        <v>20.6</v>
+      </c>
+      <c r="K10">
+        <v>5136</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="6"/>
+        <v>85.6</v>
+      </c>
+      <c r="M10">
+        <v>3900</v>
+      </c>
+      <c r="N10">
+        <v>28.4671532846715</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="7"/>
+        <v>137.00000000000017</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="12">
+        <f t="shared" si="1"/>
+        <v>1.0902777777777777E-2</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>15.7</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="O11">
+        <f>O40/2</f>
+        <v>110.00000000000044</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="12">
+        <f t="shared" si="1"/>
+        <v>8.1250000000000003E-3</v>
+      </c>
+      <c r="D12">
+        <v>1.6</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>11.7</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="2"/>
+        <v>1.8333333333333333E-2</v>
+      </c>
+      <c r="G12" s="12">
+        <f t="shared" si="3"/>
+        <v>6.3472222222222222E-2</v>
+      </c>
+      <c r="H12" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="I12">
+        <v>1584</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="5"/>
+        <v>26.4</v>
+      </c>
+      <c r="K12">
+        <v>5484</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="6"/>
+        <v>91.4</v>
+      </c>
+      <c r="M12">
+        <v>3900</v>
+      </c>
+      <c r="N12">
+        <v>29.545454545454501</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="7"/>
+        <v>132.0000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="12">
+        <f t="shared" si="1"/>
+        <v>7.013888888888889E-3</v>
+      </c>
+      <c r="D13">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>10.1</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="2"/>
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="G13" s="12">
+        <f t="shared" si="3"/>
+        <v>6.458333333333334E-2</v>
+      </c>
+      <c r="H13" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="I13">
+        <v>1680</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="K13">
+        <v>5580</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="6"/>
+        <v>93</v>
+      </c>
+      <c r="M13">
+        <v>3900</v>
+      </c>
+      <c r="N13">
+        <v>23.780487804878</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="7"/>
+        <v>164.00000000000034</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="12">
+        <f t="shared" si="1"/>
+        <v>3.8194444444444443E-3</v>
+      </c>
+      <c r="D14">
+        <v>3.4</v>
+      </c>
+      <c r="E14">
+        <f>E15+D14</f>
+        <v>5.5</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="2"/>
+        <v>2.2638888888888889E-2</v>
+      </c>
+      <c r="G14" s="12">
+        <f t="shared" si="3"/>
+        <v>6.7777777777777784E-2</v>
+      </c>
+      <c r="H14" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="I14">
+        <v>1956</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="5"/>
+        <v>32.6</v>
+      </c>
+      <c r="K14">
+        <v>5856</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="6"/>
+        <v>97.6</v>
+      </c>
+      <c r="M14">
+        <v>3900</v>
+      </c>
+      <c r="N14">
+        <v>31.451612903225801</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="7"/>
+        <v>124.00000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="12">
+        <f t="shared" si="1"/>
+        <v>1.4583333333333334E-3</v>
+      </c>
+      <c r="D15">
+        <v>1.2</v>
+      </c>
+      <c r="E15">
+        <f>E16+D15</f>
+        <v>2.1</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="2"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="G15" s="12">
+        <f t="shared" si="3"/>
+        <v>7.013888888888889E-2</v>
+      </c>
+      <c r="H15" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="I15">
+        <v>2160</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="K15">
+        <v>6060</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="6"/>
+        <v>101</v>
+      </c>
+      <c r="M15">
+        <v>3900</v>
+      </c>
+      <c r="N15">
+        <v>18.309859154929502</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="7"/>
+        <v>213.00000000000088</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="12">
+        <f t="shared" si="1"/>
+        <v>6.2500000000000001E-4</v>
+      </c>
+      <c r="D16">
+        <v>0.9</v>
+      </c>
+      <c r="E16">
+        <f>D16</f>
+        <v>0.9</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" si="2"/>
+        <v>2.5833333333333333E-2</v>
+      </c>
+      <c r="G16" s="12">
+        <f t="shared" si="3"/>
+        <v>7.0972222222222228E-2</v>
+      </c>
+      <c r="H16" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="I16">
+        <v>2232</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="5"/>
+        <v>37.200000000000003</v>
+      </c>
+      <c r="K16">
+        <v>6132</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="6"/>
+        <v>102.2</v>
+      </c>
+      <c r="M16">
+        <v>3900</v>
+      </c>
+      <c r="N16">
+        <v>21.081081081080999</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="7"/>
+        <v>185.00000000000071</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="12">
+        <f t="shared" si="1"/>
+        <v>2.2708333333333334E-2</v>
+      </c>
+      <c r="D17">
+        <v>1.2</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ref="E17:E26" si="8">E18+D17</f>
+        <v>32.700000000000003</v>
+      </c>
+      <c r="F17" s="12">
+        <f t="shared" si="2"/>
+        <v>3.7499999999999999E-3</v>
+      </c>
+      <c r="G17" s="12">
+        <f t="shared" si="3"/>
+        <v>4.8888888888888891E-2</v>
+      </c>
+      <c r="H17" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="I17">
+        <v>324</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="5"/>
+        <v>5.4</v>
+      </c>
+      <c r="K17">
+        <v>4224</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="6"/>
+        <v>70.400000000000006</v>
+      </c>
+      <c r="M17">
+        <v>3900</v>
+      </c>
+      <c r="N17">
+        <v>49.367088607594901</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="7"/>
+        <v>79.000000000000057</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="12">
+        <f t="shared" si="1"/>
+        <v>2.1874999999999999E-2</v>
+      </c>
+      <c r="D18">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="8"/>
+        <v>31.5</v>
+      </c>
+      <c r="F18" s="12">
+        <f t="shared" si="2"/>
+        <v>4.5833333333333334E-3</v>
+      </c>
+      <c r="G18" s="12">
+        <f t="shared" si="3"/>
+        <v>4.9722222222222223E-2</v>
+      </c>
+      <c r="H18" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="I18">
+        <v>396</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="5"/>
+        <v>6.6</v>
+      </c>
+      <c r="K18">
+        <v>4296</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="6"/>
+        <v>71.599999999999994</v>
+      </c>
+      <c r="M18">
+        <v>3900</v>
+      </c>
+      <c r="N18">
+        <v>56.521739130434703</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="7"/>
+        <v>69.000000000000099</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="12">
+        <f t="shared" si="1"/>
+        <v>2.0277777777777777E-2</v>
+      </c>
+      <c r="D19">
+        <v>3.2</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="8"/>
+        <v>29.2</v>
+      </c>
+      <c r="F19" s="12">
+        <f t="shared" si="2"/>
+        <v>6.1805555555555555E-3</v>
+      </c>
+      <c r="G19" s="12">
+        <f t="shared" si="3"/>
+        <v>5.1319444444444445E-2</v>
+      </c>
+      <c r="H19" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="I19">
+        <v>534</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="5"/>
+        <v>8.9</v>
+      </c>
+      <c r="K19">
+        <v>4434</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="6"/>
+        <v>73.900000000000006</v>
+      </c>
+      <c r="M19">
+        <v>3900</v>
+      </c>
+      <c r="N19">
+        <v>90.697674418604606</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="7"/>
+        <v>43.000000000000021</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="12">
+        <f t="shared" si="1"/>
+        <v>1.8055555555555554E-2</v>
+      </c>
+      <c r="D20">
+        <v>4.3</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="8"/>
+        <v>26</v>
+      </c>
+      <c r="F20" s="12">
+        <f t="shared" si="2"/>
+        <v>8.4027777777777781E-3</v>
+      </c>
+      <c r="G20" s="12">
+        <f t="shared" si="3"/>
+        <v>5.3541666666666668E-2</v>
+      </c>
+      <c r="H20" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="I20">
+        <v>726</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="5"/>
+        <v>12.1</v>
+      </c>
+      <c r="K20">
+        <v>4626</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="6"/>
+        <v>77.099999999999994</v>
+      </c>
+      <c r="M20">
+        <v>3900</v>
+      </c>
+      <c r="N20">
+        <v>30.708661417322801</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="7"/>
+        <v>127.00000000000014</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="12">
+        <f t="shared" si="1"/>
+        <v>1.5069444444444444E-2</v>
+      </c>
+      <c r="D21">
+        <v>1.2</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="8"/>
+        <v>21.7</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="O21">
+        <f>O39/2</f>
+        <v>105.00000000000028</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="12">
+        <f t="shared" si="1"/>
+        <v>1.4236111111111111E-2</v>
+      </c>
+      <c r="D22">
+        <v>2.7</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="8"/>
+        <v>20.5</v>
+      </c>
+      <c r="F22" s="12">
+        <f t="shared" si="2"/>
+        <v>1.2222222222222223E-2</v>
+      </c>
+      <c r="G22" s="12">
+        <f t="shared" si="3"/>
+        <v>5.7361111111111113E-2</v>
+      </c>
+      <c r="H22" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="I22">
+        <v>1056</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="5"/>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="K22">
+        <v>4956</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="6"/>
+        <v>82.6</v>
+      </c>
+      <c r="M22">
+        <v>3900</v>
+      </c>
+      <c r="N22">
+        <v>130</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="7"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="12">
+        <f t="shared" si="1"/>
+        <v>1.2361111111111111E-2</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="8"/>
+        <v>17.8</v>
+      </c>
+      <c r="F23" s="12">
+        <f t="shared" si="2"/>
+        <v>1.4097222222222223E-2</v>
+      </c>
+      <c r="G23" s="12">
+        <f t="shared" si="3"/>
+        <v>5.9236111111111114E-2</v>
+      </c>
+      <c r="H23" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="I23">
+        <v>1218</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="5"/>
+        <v>20.3</v>
+      </c>
+      <c r="K23">
+        <v>5118</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="6"/>
+        <v>85.3</v>
+      </c>
+      <c r="M23">
+        <v>3900</v>
+      </c>
+      <c r="N23">
+        <v>56.521739130434703</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="7"/>
+        <v>69.000000000000099</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="12">
+        <f t="shared" si="1"/>
+        <v>1.0277777777777778E-2</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="8"/>
+        <v>14.8</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="O24">
+        <f>O40/2</f>
+        <v>110.00000000000044</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="12">
+        <f t="shared" si="1"/>
+        <v>6.1111111111111114E-3</v>
+      </c>
+      <c r="D25">
+        <v>4.3</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="8"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F25" s="12">
+        <f t="shared" si="2"/>
+        <v>2.0347222222222221E-2</v>
+      </c>
+      <c r="G25" s="12">
+        <f t="shared" si="3"/>
+        <v>6.5486111111111106E-2</v>
+      </c>
+      <c r="H25" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888881E-2</v>
+      </c>
+      <c r="I25">
+        <v>1758</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="5"/>
+        <v>29.3</v>
+      </c>
+      <c r="K25">
+        <v>5658</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="6"/>
+        <v>94.3</v>
+      </c>
+      <c r="M25">
+        <v>3900</v>
+      </c>
+      <c r="N25">
+        <v>24.074074074074002</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="7"/>
+        <v>162.00000000000048</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="12">
+        <f t="shared" si="1"/>
+        <v>3.1250000000000002E-3</v>
+      </c>
+      <c r="D26">
+        <v>0.5</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="8"/>
+        <v>4.5</v>
+      </c>
+      <c r="F26" s="12">
+        <f t="shared" si="2"/>
+        <v>2.3333333333333334E-2</v>
+      </c>
+      <c r="G26" s="12">
+        <f t="shared" si="3"/>
+        <v>6.8472222222222226E-2</v>
+      </c>
+      <c r="H26" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="I26">
+        <v>2016</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="5"/>
+        <v>33.6</v>
+      </c>
+      <c r="K26">
+        <v>5916</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="6"/>
+        <v>98.6</v>
+      </c>
+      <c r="M26">
+        <v>3900</v>
+      </c>
+      <c r="N26">
+        <v>43.3333333333333</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="7"/>
+        <v>90.000000000000071</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="12">
+        <f t="shared" si="1"/>
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="D27">
+        <v>2.7</v>
+      </c>
+      <c r="E27">
+        <f>E28+D27</f>
+        <v>4</v>
+      </c>
+      <c r="F27" s="12">
+        <f t="shared" si="2"/>
+        <v>2.3680555555555555E-2</v>
+      </c>
+      <c r="G27" s="12">
+        <f t="shared" si="3"/>
+        <v>6.8819444444444447E-2</v>
+      </c>
+      <c r="H27" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="I27">
+        <v>2046</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="5"/>
+        <v>34.1</v>
+      </c>
+      <c r="K27">
+        <v>5946</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="6"/>
+        <v>99.1</v>
+      </c>
+      <c r="M27">
+        <v>3900</v>
+      </c>
+      <c r="N27">
+        <v>26.351351351351301</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="7"/>
+        <v>148.00000000000028</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="12">
+        <f t="shared" si="1"/>
+        <v>9.0277777777777784E-4</v>
+      </c>
+      <c r="D28">
+        <v>1.3</v>
+      </c>
+      <c r="E28">
+        <f>D28</f>
+        <v>1.3</v>
+      </c>
+      <c r="F28" s="12">
+        <f t="shared" si="2"/>
+        <v>2.5555555555555557E-2</v>
+      </c>
+      <c r="G28" s="12">
+        <f t="shared" si="3"/>
+        <v>7.0694444444444449E-2</v>
+      </c>
+      <c r="H28" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="I28">
+        <v>2208</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="5"/>
+        <v>36.799999999999997</v>
+      </c>
+      <c r="K28">
+        <v>6108</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="6"/>
+        <v>101.8</v>
+      </c>
+      <c r="M28">
+        <v>3900</v>
+      </c>
+      <c r="N28">
+        <v>22.807017543859601</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="7"/>
+        <v>171.00000000000037</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="12">
+        <f t="shared" si="1"/>
+        <v>2.645833333333333E-2</v>
+      </c>
+      <c r="D29">
+        <v>0.6</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ref="E29:E35" si="9">E30+D29</f>
+        <v>38.099999999999994</v>
+      </c>
+      <c r="F29" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="12">
+        <f t="shared" si="3"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="H29" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>3900</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="6"/>
+        <v>65</v>
+      </c>
+      <c r="M29">
+        <v>3900</v>
+      </c>
+      <c r="N29">
+        <v>16.25</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="7"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="12">
+        <f t="shared" si="1"/>
+        <v>2.6041666666666661E-2</v>
+      </c>
+      <c r="D30">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="9"/>
+        <v>37.499999999999993</v>
+      </c>
+      <c r="F30" s="12">
+        <f t="shared" si="2"/>
+        <v>4.1666666666666669E-4</v>
+      </c>
+      <c r="G30" s="12">
+        <f t="shared" si="3"/>
+        <v>4.5555555555555557E-2</v>
+      </c>
+      <c r="H30" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="I30">
+        <v>36</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="5"/>
+        <v>0.6</v>
+      </c>
+      <c r="K30">
+        <v>3936</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="6"/>
+        <v>65.599999999999994</v>
+      </c>
+      <c r="M30">
+        <v>3900</v>
+      </c>
+      <c r="N30">
+        <v>12.580645161290301</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="7"/>
+        <v>310.00000000000051</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="12">
+        <f t="shared" si="1"/>
+        <v>2.4444444444444442E-2</v>
+      </c>
+      <c r="D31">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="9"/>
+        <v>35.199999999999996</v>
+      </c>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="O31">
+        <f>O38/2</f>
+        <v>130.00000000000065</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="12">
+        <f t="shared" si="1"/>
+        <v>2.1597222222222219E-2</v>
+      </c>
+      <c r="D32">
+        <v>6</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="9"/>
+        <v>31.099999999999998</v>
+      </c>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="O32">
+        <f>O39/2</f>
+        <v>105.00000000000028</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="12">
+        <f t="shared" si="1"/>
+        <v>1.7430555555555553E-2</v>
+      </c>
+      <c r="D33">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="9"/>
+        <v>25.099999999999998</v>
+      </c>
+      <c r="F33" s="12">
+        <f t="shared" si="2"/>
+        <v>9.0277777777777769E-3</v>
+      </c>
+      <c r="G33" s="12">
+        <f t="shared" si="3"/>
+        <v>5.4166666666666669E-2</v>
+      </c>
+      <c r="H33" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="I33">
+        <v>780</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="K33">
+        <v>4680</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="6"/>
+        <v>78</v>
+      </c>
+      <c r="M33">
+        <v>3900</v>
+      </c>
+      <c r="N33">
+        <v>29.770992366412202</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="7"/>
+        <v>131.00000000000006</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="12">
+        <f t="shared" si="1"/>
+        <v>1.5833333333333331E-2</v>
+      </c>
+      <c r="D34">
+        <v>7.1</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="9"/>
+        <v>22.799999999999997</v>
+      </c>
+      <c r="F34" s="12">
+        <f t="shared" si="2"/>
+        <v>1.0625000000000001E-2</v>
+      </c>
+      <c r="G34" s="12">
+        <f t="shared" si="3"/>
+        <v>5.5763888888888891E-2</v>
+      </c>
+      <c r="H34" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="I34">
+        <v>918</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="5"/>
+        <v>15.3</v>
+      </c>
+      <c r="K34">
+        <v>4818</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="6"/>
+        <v>80.3</v>
+      </c>
+      <c r="M34">
+        <v>3900</v>
+      </c>
+      <c r="N34">
+        <v>20.5263157894736</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="7"/>
+        <v>190.0000000000008</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="12">
+        <f t="shared" si="1"/>
+        <v>1.0902777777777777E-2</v>
+      </c>
+      <c r="D35">
+        <v>4.8</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="9"/>
+        <v>15.7</v>
+      </c>
+      <c r="F35" s="12">
+        <f t="shared" si="2"/>
+        <v>1.5555555555555555E-2</v>
+      </c>
+      <c r="G35" s="12">
+        <f t="shared" si="3"/>
+        <v>6.0694444444444447E-2</v>
+      </c>
+      <c r="H35" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="I35">
+        <v>1344</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="5"/>
+        <v>22.4</v>
+      </c>
+      <c r="K35">
+        <v>5244</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="6"/>
+        <v>87.4</v>
+      </c>
+      <c r="M35">
+        <v>3900</v>
+      </c>
+      <c r="N35">
+        <v>29.545454545454501</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="7"/>
+        <v>132.0000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="12">
+        <f t="shared" si="1"/>
+        <v>7.5694444444444446E-3</v>
+      </c>
+      <c r="D36">
+        <v>3.7</v>
+      </c>
+      <c r="E36">
+        <f>E37+D36</f>
+        <v>10.9</v>
+      </c>
+      <c r="F36" s="12">
+        <f t="shared" si="2"/>
+        <v>1.8888888888888889E-2</v>
+      </c>
+      <c r="G36" s="12">
+        <f t="shared" si="3"/>
+        <v>6.4027777777777781E-2</v>
+      </c>
+      <c r="H36" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="I36">
+        <v>1632</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="5"/>
+        <v>27.2</v>
+      </c>
+      <c r="K36">
+        <v>5532</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="6"/>
+        <v>92.2</v>
+      </c>
+      <c r="M36">
+        <v>3900</v>
+      </c>
+      <c r="N36">
+        <v>30.46875</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="7"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="12">
+        <f t="shared" si="1"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D37">
+        <v>7.2</v>
+      </c>
+      <c r="E37">
+        <f>D37</f>
+        <v>7.2</v>
+      </c>
+      <c r="F37" s="12">
+        <f t="shared" si="2"/>
+        <v>2.1458333333333333E-2</v>
+      </c>
+      <c r="G37" s="12">
+        <f t="shared" si="3"/>
+        <v>6.6597222222222224E-2</v>
+      </c>
+      <c r="H37" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="I37">
+        <v>1854</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="5"/>
+        <v>30.9</v>
+      </c>
+      <c r="K37">
+        <v>5754</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="6"/>
+        <v>95.9</v>
+      </c>
+      <c r="M37">
+        <v>3900</v>
+      </c>
+      <c r="N37">
+        <v>55.714285714285701</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="7"/>
+        <v>70.000000000000014</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="F38" s="12">
+        <f t="shared" si="2"/>
+        <v>2.0138888888888888E-3</v>
+      </c>
+      <c r="G38" s="12">
+        <f t="shared" si="3"/>
+        <v>5.1319444444444445E-2</v>
+      </c>
+      <c r="H38" s="12">
+        <f t="shared" si="4"/>
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="I38">
+        <v>174</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="5"/>
+        <v>2.9</v>
+      </c>
+      <c r="K38">
+        <v>4434</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="6"/>
+        <v>73.900000000000006</v>
+      </c>
+      <c r="M38">
+        <v>4260</v>
+      </c>
+      <c r="N38">
+        <v>16.384615384615302</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="7"/>
+        <v>260.00000000000131</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="F39" s="12">
+        <f t="shared" si="2"/>
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="G39" s="12">
+        <f t="shared" si="3"/>
+        <v>5.6527777777777781E-2</v>
+      </c>
+      <c r="H39" s="12">
+        <f t="shared" si="4"/>
+        <v>5.1666666666666666E-2</v>
+      </c>
+      <c r="I39">
+        <v>420</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="K39">
+        <v>4884</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="6"/>
+        <v>81.400000000000006</v>
+      </c>
+      <c r="M39">
+        <v>4464</v>
+      </c>
+      <c r="N39">
+        <v>21.257142857142799</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="7"/>
+        <v>210.00000000000057</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="F40" s="12">
+        <f t="shared" si="2"/>
+        <v>1.5555555555555555E-2</v>
+      </c>
+      <c r="G40" s="12">
+        <f t="shared" si="3"/>
+        <v>6.1319444444444447E-2</v>
+      </c>
+      <c r="H40" s="12">
+        <f t="shared" si="4"/>
+        <v>4.5763888888888896E-2</v>
+      </c>
+      <c r="I40">
+        <v>1344</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="5"/>
+        <v>22.4</v>
+      </c>
+      <c r="K40">
+        <v>5298</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="6"/>
+        <v>88.3</v>
+      </c>
+      <c r="M40">
+        <v>3954</v>
+      </c>
+      <c r="N40">
+        <v>17.972727272727202</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="7"/>
+        <v>220.00000000000088</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7558AA9E-734F-4530-A613-4B8C5C34F8F1}">
+  <dimension ref="B1:H49"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45:H49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="20"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="21"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15">
+        <v>2.6388888888888885E-2</v>
+      </c>
+      <c r="D3" s="15">
+        <v>6.9444444444444444E-5</v>
+      </c>
+      <c r="E3" s="15">
+        <v>4.5208333333333336E-2</v>
+      </c>
+      <c r="F3" s="15">
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="G3" s="16">
+        <v>31.707317073170699</v>
+      </c>
+      <c r="H3" s="23">
+        <v>123.00000000000013</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="15">
+        <v>2.4166666666666659E-2</v>
+      </c>
+      <c r="D4" s="15">
+        <v>2.2916666666666667E-3</v>
+      </c>
+      <c r="E4" s="15">
+        <v>4.7430555555555552E-2</v>
+      </c>
+      <c r="F4" s="15">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="G4" s="16">
+        <v>42.391304347826001</v>
+      </c>
+      <c r="H4" s="23">
+        <v>92.000000000000185</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="15">
+        <v>2.2569444444444441E-2</v>
+      </c>
+      <c r="D5" s="15">
+        <v>3.8888888888888888E-3</v>
+      </c>
+      <c r="E5" s="15">
+        <v>4.9027777777777781E-2</v>
+      </c>
+      <c r="F5" s="15">
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="G5" s="16">
+        <v>16.182572614107801</v>
+      </c>
+      <c r="H5" s="23">
+        <v>241.00000000000122</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="15">
+        <v>2.1111111111111108E-2</v>
+      </c>
+      <c r="D6" s="15">
+        <v>5.347222222222222E-3</v>
+      </c>
+      <c r="E6" s="15">
+        <v>5.0486111111111114E-2</v>
+      </c>
+      <c r="F6" s="15">
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="G6" s="16">
+        <v>31.707317073170699</v>
+      </c>
+      <c r="H6" s="23">
+        <v>123.00000000000013</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="15">
+        <v>2.0277777777777777E-2</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="23">
+        <v>130.00000000000065</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="15">
+        <v>1.6527777777777777E-2</v>
+      </c>
+      <c r="D8" s="15">
+        <v>9.9305555555555553E-3</v>
+      </c>
+      <c r="E8" s="15">
+        <v>5.5069444444444442E-2</v>
+      </c>
+      <c r="F8" s="15">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="G8" s="16">
+        <v>18.139534883720899</v>
+      </c>
+      <c r="H8" s="23">
+        <v>215.00000000000037</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="15">
+        <v>1.4513888888888889E-2</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1.1944444444444445E-2</v>
+      </c>
+      <c r="E9" s="15">
+        <v>5.7083333333333333E-2</v>
+      </c>
+      <c r="F9" s="15">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="G9" s="16">
+        <v>15.9183673469387</v>
+      </c>
+      <c r="H9" s="23">
+        <v>245.00000000000117</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="15">
+        <v>1.2152777777777778E-2</v>
+      </c>
+      <c r="D10" s="15">
+        <v>1.4305555555555556E-2</v>
+      </c>
+      <c r="E10" s="15">
+        <v>5.9444444444444446E-2</v>
+      </c>
+      <c r="F10" s="15">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="G10" s="16">
+        <v>28.4671532846715</v>
+      </c>
+      <c r="H10" s="23">
+        <v>137.00000000000017</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1.0902777777777777E-2</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="23">
+        <v>110.00000000000044</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="15">
+        <v>8.1250000000000003E-3</v>
+      </c>
+      <c r="D12" s="15">
+        <v>1.8333333333333333E-2</v>
+      </c>
+      <c r="E12" s="15">
+        <v>6.3472222222222222E-2</v>
+      </c>
+      <c r="F12" s="15">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="G12" s="16">
+        <v>29.545454545454501</v>
+      </c>
+      <c r="H12" s="23">
+        <v>132.0000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="15">
+        <v>7.013888888888889E-3</v>
+      </c>
+      <c r="D13" s="15">
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="E13" s="15">
+        <v>6.458333333333334E-2</v>
+      </c>
+      <c r="F13" s="15">
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="G13" s="16">
+        <v>23.780487804878</v>
+      </c>
+      <c r="H13" s="23">
+        <v>164.00000000000034</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="15">
+        <v>3.8194444444444443E-3</v>
+      </c>
+      <c r="D14" s="15">
+        <v>2.2638888888888889E-2</v>
+      </c>
+      <c r="E14" s="15">
+        <v>6.7777777777777784E-2</v>
+      </c>
+      <c r="F14" s="15">
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="G14" s="16">
+        <v>31.451612903225801</v>
+      </c>
+      <c r="H14" s="23">
+        <v>124.00000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="15">
+        <v>1.4583333333333334E-3</v>
+      </c>
+      <c r="D15" s="15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E15" s="15">
+        <v>7.013888888888889E-2</v>
+      </c>
+      <c r="F15" s="15">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="G15" s="16">
+        <v>18.309859154929502</v>
+      </c>
+      <c r="H15" s="23">
+        <v>213.00000000000088</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="25">
+        <v>6.2500000000000001E-4</v>
+      </c>
+      <c r="D16" s="25">
+        <v>2.5833333333333333E-2</v>
+      </c>
+      <c r="E16" s="25">
+        <v>7.0972222222222228E-2</v>
+      </c>
+      <c r="F16" s="25">
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="G16" s="26">
+        <v>21.081081081080999</v>
+      </c>
+      <c r="H16" s="27">
+        <v>185.00000000000071</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="13"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="20"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="21"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="15">
+        <v>2.2708333333333334E-2</v>
+      </c>
+      <c r="D20" s="15">
+        <v>3.7499999999999999E-3</v>
+      </c>
+      <c r="E20" s="15">
+        <v>4.8888888888888891E-2</v>
+      </c>
+      <c r="F20" s="15">
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="G20" s="16">
+        <v>49.367088607594901</v>
+      </c>
+      <c r="H20" s="23">
+        <v>79.000000000000057</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="15">
+        <v>2.1874999999999999E-2</v>
+      </c>
+      <c r="D21" s="15">
+        <v>4.5833333333333334E-3</v>
+      </c>
+      <c r="E21" s="15">
+        <v>4.9722222222222223E-2</v>
+      </c>
+      <c r="F21" s="15">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="G21" s="16">
+        <v>56.521739130434703</v>
+      </c>
+      <c r="H21" s="23">
+        <v>69.000000000000099</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="15">
+        <v>2.0277777777777777E-2</v>
+      </c>
+      <c r="D22" s="15">
+        <v>6.1805555555555555E-3</v>
+      </c>
+      <c r="E22" s="15">
+        <v>5.1319444444444445E-2</v>
+      </c>
+      <c r="F22" s="15">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="G22" s="16">
+        <v>90.697674418604606</v>
+      </c>
+      <c r="H22" s="23">
+        <v>43.000000000000021</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="15">
+        <v>1.8055555555555554E-2</v>
+      </c>
+      <c r="D23" s="15">
+        <v>8.4027777777777781E-3</v>
+      </c>
+      <c r="E23" s="15">
+        <v>5.3541666666666668E-2</v>
+      </c>
+      <c r="F23" s="15">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="G23" s="16">
+        <v>30.708661417322801</v>
+      </c>
+      <c r="H23" s="23">
+        <v>127.00000000000014</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="15">
+        <v>1.5069444444444444E-2</v>
+      </c>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="23">
+        <v>105.00000000000028</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="15">
+        <v>1.4236111111111111E-2</v>
+      </c>
+      <c r="D25" s="15">
+        <v>1.2222222222222223E-2</v>
+      </c>
+      <c r="E25" s="15">
+        <v>5.7361111111111113E-2</v>
+      </c>
+      <c r="F25" s="15">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="G25" s="16">
+        <v>130</v>
+      </c>
+      <c r="H25" s="23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="15">
+        <v>1.2361111111111111E-2</v>
+      </c>
+      <c r="D26" s="15">
+        <v>1.4097222222222223E-2</v>
+      </c>
+      <c r="E26" s="15">
+        <v>5.9236111111111114E-2</v>
+      </c>
+      <c r="F26" s="15">
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="G26" s="16">
+        <v>56.521739130434703</v>
+      </c>
+      <c r="H26" s="23">
+        <v>69.000000000000099</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="15">
+        <v>1.0277777777777778E-2</v>
+      </c>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="23">
+        <v>110.00000000000044</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="15">
+        <v>6.1111111111111114E-3</v>
+      </c>
+      <c r="D28" s="15">
+        <v>2.0347222222222221E-2</v>
+      </c>
+      <c r="E28" s="15">
+        <v>6.5486111111111106E-2</v>
+      </c>
+      <c r="F28" s="15">
+        <v>4.5138888888888881E-2</v>
+      </c>
+      <c r="G28" s="16">
+        <v>24.074074074074002</v>
+      </c>
+      <c r="H28" s="23">
+        <v>162.00000000000048</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="15">
+        <v>3.1250000000000002E-3</v>
+      </c>
+      <c r="D29" s="15">
+        <v>2.3333333333333334E-2</v>
+      </c>
+      <c r="E29" s="15">
+        <v>6.8472222222222226E-2</v>
+      </c>
+      <c r="F29" s="15">
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="G29" s="16">
+        <v>43.3333333333333</v>
+      </c>
+      <c r="H29" s="23">
+        <v>90.000000000000071</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="15">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="D30" s="15">
+        <v>2.3680555555555555E-2</v>
+      </c>
+      <c r="E30" s="15">
+        <v>6.8819444444444447E-2</v>
+      </c>
+      <c r="F30" s="15">
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="G30" s="16">
+        <v>26.351351351351301</v>
+      </c>
+      <c r="H30" s="23">
+        <v>148.00000000000028</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="25">
+        <v>9.0277777777777784E-4</v>
+      </c>
+      <c r="D31" s="25">
+        <v>2.5555555555555557E-2</v>
+      </c>
+      <c r="E31" s="25">
+        <v>7.0694444444444449E-2</v>
+      </c>
+      <c r="F31" s="25">
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="G31" s="26">
+        <v>22.807017543859601</v>
+      </c>
+      <c r="H31" s="27">
+        <v>171.00000000000037</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="13"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H33" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="20"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="21"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="15">
+        <v>2.645833333333333E-2</v>
+      </c>
+      <c r="D35" s="15">
+        <v>0</v>
+      </c>
+      <c r="E35" s="15">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="F35" s="15">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="G35" s="16">
+        <v>16.25</v>
+      </c>
+      <c r="H35" s="23">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="15">
+        <v>2.6041666666666661E-2</v>
+      </c>
+      <c r="D36" s="15">
+        <v>4.1666666666666669E-4</v>
+      </c>
+      <c r="E36" s="15">
+        <v>4.5555555555555557E-2</v>
+      </c>
+      <c r="F36" s="15">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="G36" s="16">
+        <v>12.580645161290301</v>
+      </c>
+      <c r="H36" s="23">
+        <v>310.00000000000051</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="15">
+        <v>2.4444444444444442E-2</v>
+      </c>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="23">
+        <v>130.00000000000065</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="15">
+        <v>2.1597222222222219E-2</v>
+      </c>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="23">
+        <v>105.00000000000028</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="15">
+        <v>1.7430555555555553E-2</v>
+      </c>
+      <c r="D39" s="15">
+        <v>9.0277777777777769E-3</v>
+      </c>
+      <c r="E39" s="15">
+        <v>5.4166666666666669E-2</v>
+      </c>
+      <c r="F39" s="15">
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="G39" s="16">
+        <v>29.770992366412202</v>
+      </c>
+      <c r="H39" s="23">
+        <v>131.00000000000006</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="15">
+        <v>1.5833333333333331E-2</v>
+      </c>
+      <c r="D40" s="15">
+        <v>1.0625000000000001E-2</v>
+      </c>
+      <c r="E40" s="15">
+        <v>5.5763888888888891E-2</v>
+      </c>
+      <c r="F40" s="15">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="G40" s="16">
+        <v>20.5263157894736</v>
+      </c>
+      <c r="H40" s="23">
+        <v>190.0000000000008</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" s="15">
+        <v>1.0902777777777777E-2</v>
+      </c>
+      <c r="D41" s="15">
+        <v>1.5555555555555555E-2</v>
+      </c>
+      <c r="E41" s="15">
+        <v>6.0694444444444447E-2</v>
+      </c>
+      <c r="F41" s="15">
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="G41" s="16">
+        <v>29.545454545454501</v>
+      </c>
+      <c r="H41" s="23">
+        <v>132.0000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="15">
+        <v>7.5694444444444446E-3</v>
+      </c>
+      <c r="D42" s="15">
+        <v>1.8888888888888889E-2</v>
+      </c>
+      <c r="E42" s="15">
+        <v>6.4027777777777781E-2</v>
+      </c>
+      <c r="F42" s="15">
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="G42" s="16">
+        <v>30.46875</v>
+      </c>
+      <c r="H42" s="23">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="25">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D43" s="25">
+        <v>2.1458333333333333E-2</v>
+      </c>
+      <c r="E43" s="25">
+        <v>6.6597222222222224E-2</v>
+      </c>
+      <c r="F43" s="25">
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="G43" s="26">
+        <v>55.714285714285701</v>
+      </c>
+      <c r="H43" s="27">
+        <v>70.000000000000014</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="13"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H45" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="20"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="21"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15">
+        <v>2.0138888888888888E-3</v>
+      </c>
+      <c r="E47" s="15">
+        <v>5.1319444444444445E-2</v>
+      </c>
+      <c r="F47" s="15">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="G47" s="16">
+        <v>16.384615384615302</v>
+      </c>
+      <c r="H47" s="23">
+        <v>260.00000000000131</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="E48" s="15">
+        <v>5.6527777777777781E-2</v>
+      </c>
+      <c r="F48" s="15">
+        <v>5.1666666666666666E-2</v>
+      </c>
+      <c r="G48" s="16">
+        <v>21.257142857142799</v>
+      </c>
+      <c r="H48" s="23">
+        <v>210.00000000000057</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25">
+        <v>1.5555555555555555E-2</v>
+      </c>
+      <c r="E49" s="25">
+        <v>6.1319444444444447E-2</v>
+      </c>
+      <c r="F49" s="25">
+        <v>4.5763888888888896E-2</v>
+      </c>
+      <c r="G49" s="26">
+        <v>17.972727272727202</v>
+      </c>
+      <c r="H49" s="27">
+        <v>220.00000000000088</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
copy konstruktor typ vozidla
</commit_message>
<xml_diff>
--- a/Generovanie kodu.xlsx
+++ b/Generovanie kodu.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrej Beliančin\Projects\DIS-SEM-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4059B440-8BEF-4DC1-AEAB-04818809CDF8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A124E790-1005-4E10-AEA3-8F2CA1D2DD86}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CAA8F1F5-8409-4114-88BB-3627D0CE125A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{CAA8F1F5-8409-4114-88BB-3627D0CE125A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
     <sheet name="Hárok2" sheetId="2" r:id="rId2"/>
     <sheet name="Hárok3" sheetId="3" r:id="rId3"/>
     <sheet name="Hárok4" sheetId="4" r:id="rId4"/>
+    <sheet name="Hárok5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="182">
   <si>
     <t>Linka A</t>
   </si>
@@ -304,6 +305,282 @@
   </si>
   <si>
     <t>Linka A 2 krat</t>
+  </si>
+  <si>
+    <t>Linka C 2 krat</t>
+  </si>
+  <si>
+    <t>Linka B 2 krat</t>
+  </si>
+  <si>
+    <t>Linka B 3 krat</t>
+  </si>
+  <si>
+    <t>´=6*60+64</t>
+  </si>
+  <si>
+    <t>Počet cestujúcich</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4720,3521 ±,6574 </t>
+  </si>
+  <si>
+    <t>Priemerný čas čakania na zastávke</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 597,5431 ±,4289 </t>
+  </si>
+  <si>
+    <t>Percento ľudí prichádzajúcich po začiatku zapasu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6,2842 ±,0112 </t>
+  </si>
+  <si>
+    <t>Priemerný zisk minibusov</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ,0000 ±,0000 </t>
+  </si>
+  <si>
+    <t>Náklady konfigurácie</t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 1, linka: A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2,0000 ±,0000 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 1, linka: A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 98,1007 ±,0432 </t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 2, linka: A</t>
+  </si>
+  <si>
+    <t>Vyťaženie V 2, linka: A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 66,6992 ±,0530 </t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 3, linka: A</t>
+  </si>
+  <si>
+    <t>Vyťaženie V 3, linka: A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 94,7307 ±,0617 </t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 4, linka: A</t>
+  </si>
+  <si>
+    <t>Vyťaženie V 4, linka: A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 74,0672 ±,1325 </t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 5, linka: A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,9744 ±,0009 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 5, linka: A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 59,9057 ±,3278 </t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 6, linka: A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,8318 ±,0011 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 6, linka: A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 100,0000 ±,0000 </t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 7, linka: A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,4396 ±,0011 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 7, linka: A</t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 8, linka: A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,3720 ±,0011 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 8, linka: A</t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 9, linka: A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,2835 ±,0011 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 9, linka: A</t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 10, linka: B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2,6922 ±,0013 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 10, linka: B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 99,3165 ±,0254 </t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 11, linka: B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2,5103 ±,0013 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 11, linka: B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 87,2172 ±,0749 </t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 12, linka: B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2,3875 ±,0013 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 12, linka: B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 95,0154 ±,0711 </t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 13, linka: B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2,2206 ±,0013 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 13, linka: B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 82,5365 ±,1556 </t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 14, linka: B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,9982 ±,0001 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 14, linka: B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 57,0766 ±,2840 </t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 15, linka: C</t>
+  </si>
+  <si>
+    <t>Vyťaženie V 15, linka: C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 62,6183 ±,0430 </t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 16, linka: C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,9698 ±,0010 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 16, linka: C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 65,5527 ±,2887 </t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 17, linka: C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,8290 ±,0011 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 17, linka: C</t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 18, linka: C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,6757 ±,0011 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 18, linka: C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 99,4281 ±,0389 </t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 19, linka: C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,3487 ±,0011 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 19, linka: C</t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 20, linka: C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,1727 ±,0011 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 20, linka: C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 99,9977 ±,0022 </t>
+  </si>
+  <si>
+    <t>Priemerný počet jázd V. 21, linka: C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,0251 ±,0002 </t>
+  </si>
+  <si>
+    <t>Vyťaženie V 21, linka: C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 99,6629 ±,0316 </t>
+  </si>
+  <si>
+    <t>90%-ný ľavý interval spoľahlivosti</t>
+  </si>
+  <si>
+    <t>90%-ný pravý interval spoľahlivosti</t>
+  </si>
+  <si>
+    <t>Názov štatistiky</t>
+  </si>
+  <si>
+    <t>Hodnota</t>
   </si>
 </sst>
 </file>
@@ -313,7 +590,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,6 +607,21 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -567,7 +859,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -608,6 +900,31 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -1985,10 +2302,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C15344-21F8-4E67-A098-0EABFA05ED44}">
-  <dimension ref="A1:X49"/>
+  <dimension ref="A1:X68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W35" sqref="W35"/>
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4116,6 +4433,10 @@
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <f>545000-320000</f>
+        <v>225000</v>
+      </c>
       <c r="G45" t="s">
         <v>89</v>
       </c>
@@ -4147,7 +4468,11 @@
         <v>2.6388888888888889E-2</v>
       </c>
     </row>
-    <row r="49" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <f>12*60</f>
+        <v>720</v>
+      </c>
       <c r="I49" s="12">
         <f>$C$1-I48</f>
         <v>8.4027777777777729E-3</v>
@@ -4155,6 +4480,149 @@
       <c r="J49" s="12">
         <f>$C$1-J48</f>
         <v>5.215277777777777E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>90</v>
+      </c>
+      <c r="H51">
+        <v>38.1</v>
+      </c>
+    </row>
+    <row r="52" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H52">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H53">
+        <v>38.1</v>
+      </c>
+    </row>
+    <row r="54" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H54">
+        <f>SUM(H51:H53)</f>
+        <v>106.19999999999999</v>
+      </c>
+      <c r="I54" s="12">
+        <f>H54/(86400 / 60)</f>
+        <v>7.3749999999999996E-2</v>
+      </c>
+      <c r="J54" s="12">
+        <f>H53/(86400 / 60)</f>
+        <v>2.6458333333333334E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>93</v>
+      </c>
+      <c r="I55" s="12">
+        <f>$C$1-I54</f>
+        <v>4.7916666666666663E-3</v>
+      </c>
+      <c r="J55" s="12">
+        <f>$C$1-J54</f>
+        <v>5.2083333333333329E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>91</v>
+      </c>
+      <c r="H57">
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="58" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H58">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H59">
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="60" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H60">
+        <f>SUM(H57:H59)</f>
+        <v>75.400000000000006</v>
+      </c>
+      <c r="I60" s="12">
+        <f>H60/(86400 / 60)</f>
+        <v>5.2361111111111115E-2</v>
+      </c>
+      <c r="J60" s="12">
+        <f>H59/(86400 / 60)</f>
+        <v>2.2708333333333334E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <f>37*60+42</f>
+        <v>2262</v>
+      </c>
+      <c r="I61" s="12">
+        <f>$C$1-I60</f>
+        <v>2.6180555555555547E-2</v>
+      </c>
+      <c r="J61" s="12">
+        <f>$C$1-J60</f>
+        <v>5.5833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G62" t="s">
+        <v>92</v>
+      </c>
+      <c r="H62">
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H63">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H64">
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="65" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H65">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H66">
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="67" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H67">
+        <f>SUM(H62:H66)</f>
+        <v>118.10000000000001</v>
+      </c>
+      <c r="I67" s="12">
+        <f>H67/(86400 / 60)</f>
+        <v>8.20138888888889E-2</v>
+      </c>
+      <c r="J67" s="12">
+        <f>H64/(86400 / 60)</f>
+        <v>2.2708333333333334E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="I68" s="12">
+        <f>$C$1-I67</f>
+        <v>-3.4722222222222376E-3</v>
+      </c>
+      <c r="J68" s="12">
+        <f>$C$1-J67</f>
+        <v>5.5833333333333332E-2</v>
       </c>
     </row>
   </sheetData>
@@ -6027,8 +6495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7558AA9E-734F-4530-A613-4B8C5C34F8F1}">
   <dimension ref="B1:H49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45:H49"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7045,4 +7513,709 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20CF393B-61F8-4FE9-A2A4-B7C7E9A0B0BC}">
+  <dimension ref="B3:E54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="44.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="28"/>
+    </row>
+    <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="40"/>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="30">
+        <v>10770000</v>
+      </c>
+      <c r="D8" s="30"/>
+      <c r="E8" s="31"/>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="30">
+        <v>4719.6947</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="31">
+        <v>4721.0095000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="30">
+        <v>597.11419999999998</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="31">
+        <v>597.97199999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="30">
+        <v>6.2729999999999997</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="31">
+        <v>6.2953999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="30">
+        <v>0</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="30">
+        <v>2</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="30">
+        <v>98.057500000000005</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="31">
+        <v>98.144000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="30">
+        <v>2</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="30">
+        <v>66.646199999999993</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" s="31">
+        <v>66.752200000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="30">
+        <v>2</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="30">
+        <v>94.6691</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="31">
+        <v>94.792400000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="30">
+        <v>2</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="C20" s="30">
+        <v>73.934700000000007</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="31">
+        <v>74.199700000000007</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="30">
+        <v>1.9735</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" s="31">
+        <v>1.9752000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="30">
+        <v>59.577800000000003</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="31">
+        <v>60.233499999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="30">
+        <v>1.8307</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" s="31">
+        <v>1.833</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" s="30">
+        <v>100</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C25" s="30">
+        <v>1.4383999999999999</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="E25" s="31">
+        <v>1.4407000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" s="30">
+        <v>100</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" s="31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="30">
+        <v>1.3709</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="31">
+        <v>1.3732</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C28" s="30">
+        <v>100</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="E28" s="31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="30">
+        <v>1.2824</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="31">
+        <v>1.2847</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="C30" s="30">
+        <v>100</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="E30" s="31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="C31" s="30">
+        <v>2.6909000000000001</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="E31" s="31">
+        <v>2.6934999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" s="30">
+        <v>99.2911</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" s="31">
+        <v>99.341800000000006</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" s="30">
+        <v>2.5089999999999999</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="E33" s="31">
+        <v>2.5116000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" s="30">
+        <v>87.142300000000006</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" s="31">
+        <v>87.292100000000005</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B35" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="C35" s="30">
+        <v>2.3860999999999999</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E35" s="31">
+        <v>2.3887999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" s="30">
+        <v>94.944400000000002</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="E36" s="31">
+        <v>95.086500000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="C37" s="30">
+        <v>2.2191999999999998</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" s="31">
+        <v>2.2219000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" s="30">
+        <v>82.381</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="E38" s="31">
+        <v>82.692099999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="C39" s="30">
+        <v>1.9981</v>
+      </c>
+      <c r="D39" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="E39" s="31">
+        <v>1.9983</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" s="30">
+        <v>56.792700000000004</v>
+      </c>
+      <c r="D40" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" s="31">
+        <v>57.360599999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="30">
+        <v>2</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E41" s="31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" s="30">
+        <v>62.575400000000002</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="E42" s="31">
+        <v>62.661299999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="C43" s="30">
+        <v>1.9686999999999999</v>
+      </c>
+      <c r="D43" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="E43" s="31">
+        <v>1.9708000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="C44" s="30">
+        <v>65.263999999999996</v>
+      </c>
+      <c r="D44" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="E44" s="31">
+        <v>65.841399999999993</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C45" s="30">
+        <v>1.8279000000000001</v>
+      </c>
+      <c r="D45" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="E45" s="31">
+        <v>1.8302</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" s="30">
+        <v>100</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="E46" s="31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="C47" s="30">
+        <v>1.6746000000000001</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="E47" s="31">
+        <v>1.6768000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B48" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="C48" s="30">
+        <v>99.389200000000002</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="E48" s="31">
+        <v>99.466899999999995</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="C49" s="30">
+        <v>1.3475999999999999</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="E49" s="31">
+        <v>1.3498000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="C50" s="30">
+        <v>100</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="E50" s="31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B51" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="C51" s="30">
+        <v>1.1716</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="E51" s="31">
+        <v>1.1738999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B52" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="C52" s="30">
+        <v>99.995500000000007</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="E52" s="31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B53" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="C53" s="30">
+        <v>1.0248999999999999</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="E53" s="31">
+        <v>1.0254000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="C54" s="33">
+        <v>99.631299999999996</v>
+      </c>
+      <c r="D54" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="E54" s="34">
+        <v>99.694599999999994</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="D6:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>